<commit_message>
Update example for multi-state scheme
Update example in multi-state scheme tab to represent two different kinetic schemes, one described by relaxation times for the complete system, and one described by transition rate constants for the connections between three states.
</commit_message>
<xml_diff>
--- a/example/xls_example.xlsx
+++ b/example/xls_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\20230515_excel2mmcif_template_coloring\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\flr2mmcif_devel\20240426_modification_of_example\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61A682C-9127-432E-94D3-B08A2DC0AFAB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D4213-D746-41C4-8BD6-9C2A54BD8AC8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="730" firstSheet="14" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="1189">
   <si>
     <t>Model number</t>
   </si>
@@ -3005,12 +3005,6 @@
     <t>cluster 2</t>
   </si>
   <si>
-    <t>Ensemble for A</t>
-  </si>
-  <si>
-    <t>Ensemble for B</t>
-  </si>
-  <si>
     <t>Description of Sample preparation and Measurement conditions</t>
   </si>
   <si>
@@ -3533,27 +3527,9 @@
     <t xml:space="preserve">FRET analysis ID. This is used for connection to multi-state schemes. While the ID in the first column specifies a distance restraint, multiple distance restraints could be obtained from the same FRET analysis. For a FRET analysis, the settings (such as correction parameters) should be the same. This is not checked. </t>
   </si>
   <si>
-    <t>Scheme 1</t>
-  </si>
-  <si>
-    <t>Scheme 2</t>
-  </si>
-  <si>
-    <t>Scheme 3</t>
-  </si>
-  <si>
     <t>An ID for the multi-state scheme - this connects multiple connectivities. Different schemes could e.g. describe different conditions, such as with and without ligand</t>
   </si>
   <si>
-    <t>RelaxationTime1</t>
-  </si>
-  <si>
-    <t>RelaxationTime3</t>
-  </si>
-  <si>
-    <t>RelaxationTime4</t>
-  </si>
-  <si>
     <t>milliseconds</t>
   </si>
   <si>
@@ -3569,9 +3545,6 @@
     <t>equilibrium constant is determined from another method not listed</t>
   </si>
   <si>
-    <t>EQ_DummyUnit</t>
-  </si>
-  <si>
     <t>FLR_FRET_analysis_id</t>
   </si>
   <si>
@@ -3627,6 +3600,60 @@
   </si>
   <si>
     <t>Dataset Type</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>tr1 - first relaxation time for the system</t>
+  </si>
+  <si>
+    <t>tr2 - second relaxation time for the system</t>
+  </si>
+  <si>
+    <t>tr3 - third relaxation time for the system</t>
+  </si>
+  <si>
+    <t>k12 - Kinetic transition rate constant for connection betwen C1 and C2</t>
+  </si>
+  <si>
+    <t>k32 - Kinetic transition rate constant for connection betwen C3 and C2</t>
+  </si>
+  <si>
+    <t>k23 - Kinetic transition rate constant for connection betwen C2 and C3</t>
+  </si>
+  <si>
+    <t>Relaxation times</t>
+  </si>
+  <si>
+    <t>Relaxation times for the complete scheme from FCS</t>
+  </si>
+  <si>
+    <t>Transition rate constants</t>
+  </si>
+  <si>
+    <t>Transition rate constants between states</t>
+  </si>
+  <si>
+    <t>Ensemble for C1</t>
+  </si>
+  <si>
+    <t>Ensemble for C2</t>
+  </si>
+  <si>
+    <t>k12</t>
+  </si>
+  <si>
+    <t>k23</t>
+  </si>
+  <si>
+    <t>k32</t>
   </si>
 </sst>
 </file>
@@ -4545,15 +4572,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4635,7 +4662,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4907,7 +4934,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5095,7 +5122,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5213,8 +5240,8 @@
       <c r="A5" s="85">
         <v>1</v>
       </c>
-      <c r="B5" s="85">
-        <v>1</v>
+      <c r="B5" s="85" t="s">
+        <v>1171</v>
       </c>
       <c r="C5" s="85">
         <v>1</v>
@@ -5229,7 +5256,7 @@
         <v>963</v>
       </c>
       <c r="G5" s="85" t="s">
-        <v>908</v>
+        <v>1171</v>
       </c>
       <c r="I5" s="85">
         <v>1</v>
@@ -5242,14 +5269,14 @@
       <c r="A6" s="85">
         <v>2</v>
       </c>
-      <c r="B6" s="85">
-        <v>2</v>
+      <c r="B6" s="85" t="s">
+        <v>1172</v>
       </c>
       <c r="C6" s="85">
         <v>2</v>
       </c>
       <c r="D6" s="85">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="E6" s="85">
         <v>0.05</v>
@@ -5258,7 +5285,7 @@
         <v>963</v>
       </c>
       <c r="G6" s="85" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="I6" s="85">
         <v>2</v>
@@ -5268,7 +5295,30 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F7" s="65"/>
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="111" t="s">
+        <v>963</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J7" t="s">
+        <v>964</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5287,8 +5337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3412B954-CC29-49CA-9B82-95A52B6CE843}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5317,7 +5367,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B1" s="111"/>
       <c r="E1" s="111"/>
@@ -5332,79 +5382,79 @@
         <v>641</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="C2" s="119" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D2" s="120" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E2" s="118" t="s">
         <v>1082</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="F2" s="119" t="s">
         <v>1083</v>
       </c>
-      <c r="E2" s="118" t="s">
+      <c r="G2" s="119" t="s">
         <v>1084</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="H2" s="120" t="s">
         <v>1085</v>
       </c>
-      <c r="G2" s="119" t="s">
+      <c r="I2" s="118" t="s">
         <v>1086</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="J2" s="119" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K2" s="119" t="s">
         <v>1087</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="L2" s="119" t="s">
         <v>1088</v>
       </c>
-      <c r="J2" s="119" t="s">
+      <c r="M2" s="119" t="s">
+        <v>1089</v>
+      </c>
+      <c r="N2" s="119" t="s">
+        <v>1090</v>
+      </c>
+      <c r="O2" s="120" t="s">
+        <v>1091</v>
+      </c>
+      <c r="P2" s="118" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Q2" s="121" t="s">
+        <v>1093</v>
+      </c>
+      <c r="R2" s="121" t="s">
+        <v>1094</v>
+      </c>
+      <c r="S2" s="119" t="s">
+        <v>1095</v>
+      </c>
+      <c r="T2" s="119" t="s">
+        <v>1096</v>
+      </c>
+      <c r="U2" s="121" t="s">
+        <v>1097</v>
+      </c>
+      <c r="V2" s="119" t="s">
+        <v>1098</v>
+      </c>
+      <c r="W2" s="118" t="s">
+        <v>1099</v>
+      </c>
+      <c r="X2" s="119" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Y2" s="119" t="s">
+        <v>1100</v>
+      </c>
+      <c r="Z2" s="120" t="s">
         <v>1162</v>
-      </c>
-      <c r="K2" s="119" t="s">
-        <v>1089</v>
-      </c>
-      <c r="L2" s="119" t="s">
-        <v>1090</v>
-      </c>
-      <c r="M2" s="119" t="s">
-        <v>1091</v>
-      </c>
-      <c r="N2" s="119" t="s">
-        <v>1092</v>
-      </c>
-      <c r="O2" s="120" t="s">
-        <v>1093</v>
-      </c>
-      <c r="P2" s="118" t="s">
-        <v>1094</v>
-      </c>
-      <c r="Q2" s="121" t="s">
-        <v>1095</v>
-      </c>
-      <c r="R2" s="121" t="s">
-        <v>1096</v>
-      </c>
-      <c r="S2" s="119" t="s">
-        <v>1097</v>
-      </c>
-      <c r="T2" s="119" t="s">
-        <v>1098</v>
-      </c>
-      <c r="U2" s="121" t="s">
-        <v>1099</v>
-      </c>
-      <c r="V2" s="119" t="s">
-        <v>1100</v>
-      </c>
-      <c r="W2" s="118" t="s">
-        <v>1101</v>
-      </c>
-      <c r="X2" s="119" t="s">
-        <v>1170</v>
-      </c>
-      <c r="Y2" s="119" t="s">
-        <v>1102</v>
-      </c>
-      <c r="Z2" s="120" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -5412,151 +5462,151 @@
         <v>129</v>
       </c>
       <c r="B3" s="122" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D3" s="123" t="s">
         <v>1103</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="E3" s="124" t="s">
         <v>1104</v>
       </c>
-      <c r="D3" s="123" t="s">
+      <c r="F3" s="81" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G3" s="81" t="s">
         <v>1105</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="H3" s="123" t="s">
         <v>1106</v>
       </c>
-      <c r="F3" s="81" t="s">
-        <v>1106</v>
-      </c>
-      <c r="G3" s="81" t="s">
+      <c r="I3" s="122" t="s">
         <v>1107</v>
       </c>
-      <c r="H3" s="123" t="s">
+      <c r="K3" s="81" t="s">
         <v>1108</v>
       </c>
-      <c r="I3" s="122" t="s">
+      <c r="L3" s="81" t="s">
         <v>1109</v>
       </c>
-      <c r="K3" s="81" t="s">
+      <c r="M3" s="81" t="s">
         <v>1110</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="N3" s="81" t="s">
         <v>1111</v>
       </c>
-      <c r="M3" s="81" t="s">
+      <c r="O3" s="123" t="s">
         <v>1112</v>
       </c>
-      <c r="N3" s="81" t="s">
+      <c r="P3" s="122" t="s">
         <v>1113</v>
       </c>
-      <c r="O3" s="123" t="s">
+      <c r="Q3" s="81" t="s">
         <v>1114</v>
       </c>
-      <c r="P3" s="122" t="s">
+      <c r="R3" s="81" t="s">
         <v>1115</v>
       </c>
-      <c r="Q3" s="81" t="s">
+      <c r="S3" s="81" t="s">
         <v>1116</v>
       </c>
-      <c r="R3" s="81" t="s">
+      <c r="T3" s="81" t="s">
         <v>1117</v>
       </c>
-      <c r="S3" s="81" t="s">
+      <c r="U3" s="81" t="s">
         <v>1118</v>
       </c>
-      <c r="T3" s="81" t="s">
+      <c r="V3" s="81" t="s">
         <v>1119</v>
       </c>
-      <c r="U3" s="81" t="s">
+      <c r="W3" s="122" t="s">
         <v>1120</v>
       </c>
-      <c r="V3" s="81" t="s">
+      <c r="Y3" s="81" t="s">
         <v>1121</v>
-      </c>
-      <c r="W3" s="122" t="s">
-        <v>1122</v>
-      </c>
-      <c r="Y3" s="81" t="s">
-        <v>1123</v>
       </c>
       <c r="Z3" s="123"/>
     </row>
     <row r="4" spans="1:26" s="70" customFormat="1" ht="48" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>1124</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="D4" s="126" t="s">
         <v>1125</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="127" t="s">
         <v>1126</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="F4" s="16" t="s">
         <v>1127</v>
       </c>
-      <c r="E4" s="127" t="s">
+      <c r="G4" s="16" t="s">
         <v>1128</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="H4" s="126" t="s">
         <v>1129</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="I4" s="125" t="s">
         <v>1130</v>
       </c>
-      <c r="H4" s="126" t="s">
+      <c r="J4" s="16" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>1131</v>
       </c>
-      <c r="I4" s="125" t="s">
+      <c r="L4" s="16" t="s">
         <v>1132</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="M4" s="16" t="s">
+        <v>1133</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>1134</v>
+      </c>
+      <c r="O4" s="126" t="s">
+        <v>1135</v>
+      </c>
+      <c r="P4" s="125" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>1137</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>1138</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>1139</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>1140</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>1141</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>1142</v>
+      </c>
+      <c r="W4" s="125" t="s">
+        <v>1143</v>
+      </c>
+      <c r="X4" s="16" t="s">
         <v>1163</v>
       </c>
-      <c r="K4" s="16" t="s">
-        <v>1133</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>1134</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>1135</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>1136</v>
-      </c>
-      <c r="O4" s="126" t="s">
-        <v>1137</v>
-      </c>
-      <c r="P4" s="125" t="s">
-        <v>1138</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>1139</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>1140</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>1141</v>
-      </c>
-      <c r="T4" s="16" t="s">
-        <v>1142</v>
-      </c>
-      <c r="U4" s="16" t="s">
-        <v>1143</v>
-      </c>
-      <c r="V4" s="16" t="s">
+      <c r="Y4" s="16" t="s">
         <v>1144</v>
       </c>
-      <c r="W4" s="125" t="s">
-        <v>1145</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>1172</v>
-      </c>
-      <c r="Y4" s="16" t="s">
-        <v>1146</v>
-      </c>
       <c r="Z4" s="126" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -5567,31 +5617,31 @@
         <v>1</v>
       </c>
       <c r="C5" s="111" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E5" s="130">
-        <v>1</v>
-      </c>
-      <c r="F5" s="111">
-        <v>2</v>
+        <v>1180</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E5" s="130" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F5" s="111" t="s">
+        <v>1172</v>
       </c>
       <c r="H5" s="111">
         <v>1</v>
       </c>
       <c r="I5" s="130" t="s">
-        <v>1152</v>
+        <v>1174</v>
       </c>
       <c r="J5" s="81" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="K5" s="45">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="L5" s="111" t="s">
-        <v>1156</v>
-      </c>
-      <c r="M5" s="111">
-        <v>0.5</v>
+        <v>1147</v>
       </c>
       <c r="N5" s="111">
         <v>1</v>
@@ -5600,28 +5650,9 @@
         <v>1</v>
       </c>
       <c r="P5" s="130"/>
-      <c r="Q5" s="45">
-        <v>20</v>
-      </c>
-      <c r="R5" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="S5" s="111" t="s">
-        <v>1157</v>
-      </c>
-      <c r="T5" s="111" t="s">
-        <v>1160</v>
-      </c>
-      <c r="U5" s="111">
-        <v>1</v>
-      </c>
-      <c r="V5" s="111">
-        <v>1</v>
-      </c>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
       <c r="W5" s="74">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="111">
         <v>1</v>
       </c>
     </row>
@@ -5633,34 +5664,41 @@
         <v>1</v>
       </c>
       <c r="C6" s="111" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E6" s="74">
-        <v>2</v>
-      </c>
-      <c r="F6" s="111">
-        <v>1</v>
+        <v>1180</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E6" s="74" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F6" s="111" t="s">
+        <v>1173</v>
       </c>
       <c r="H6" s="111">
         <v>1</v>
       </c>
-      <c r="Q6" s="111">
-        <v>150</v>
-      </c>
-      <c r="R6" s="45">
-        <v>10</v>
-      </c>
-      <c r="S6" s="111" t="s">
-        <v>1158</v>
-      </c>
-      <c r="U6" s="111">
+      <c r="I6" s="74" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J6" s="81" t="s">
+        <v>1160</v>
+      </c>
+      <c r="K6" s="111">
+        <v>70</v>
+      </c>
+      <c r="L6" s="111" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N6" s="111">
         <v>1</v>
       </c>
-      <c r="V6" s="111">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="111">
-        <v>2</v>
+      <c r="O6" s="111">
+        <v>1</v>
+      </c>
+      <c r="R6" s="45"/>
+      <c r="W6" s="74">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -5668,27 +5706,42 @@
         <v>3</v>
       </c>
       <c r="B7" s="74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="111" t="s">
-        <v>1149</v>
+        <v>1180</v>
+      </c>
+      <c r="D7" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E7" s="74" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F7" s="111" t="s">
+        <v>1172</v>
       </c>
       <c r="H7" s="111">
         <v>1</v>
       </c>
       <c r="I7" s="74" t="s">
-        <v>1153</v>
+        <v>1176</v>
       </c>
       <c r="J7" s="81" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="K7" s="111">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="L7" s="111" t="s">
-        <v>1156</v>
+        <v>1147</v>
       </c>
       <c r="N7" s="111">
+        <v>1</v>
+      </c>
+      <c r="O7" s="111">
+        <v>1</v>
+      </c>
+      <c r="W7" s="74">
         <v>1</v>
       </c>
     </row>
@@ -5700,27 +5753,36 @@
         <v>2</v>
       </c>
       <c r="C8" s="111" t="s">
-        <v>1149</v>
+        <v>1182</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>1186</v>
       </c>
       <c r="H8" s="111">
         <v>1</v>
       </c>
-      <c r="I8" s="74" t="s">
-        <v>1154</v>
-      </c>
-      <c r="J8" s="81" t="s">
-        <v>1169</v>
-      </c>
-      <c r="K8" s="111">
-        <v>125</v>
-      </c>
-      <c r="L8" s="111" t="s">
-        <v>1155</v>
-      </c>
-      <c r="N8" s="111">
+      <c r="P8" s="74" t="s">
+        <v>1177</v>
+      </c>
+      <c r="Q8" s="111">
+        <v>20</v>
+      </c>
+      <c r="U8" s="111">
         <v>1</v>
       </c>
-      <c r="W8" s="74">
+      <c r="V8" s="111">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="111">
         <v>2</v>
       </c>
     </row>
@@ -5729,22 +5791,40 @@
         <v>5</v>
       </c>
       <c r="B9" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="111" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E9" s="74">
+        <v>1182</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H9" s="111">
         <v>1</v>
       </c>
+      <c r="P9" s="74" t="s">
+        <v>1179</v>
+      </c>
       <c r="Q9" s="111">
-        <v>14</v>
-      </c>
-      <c r="R9" s="111">
-        <v>5</v>
-      </c>
-      <c r="S9" s="111" t="s">
-        <v>1159</v>
+        <v>150</v>
+      </c>
+      <c r="U9" s="111">
+        <v>1</v>
+      </c>
+      <c r="V9" s="111">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="111">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -5752,40 +5832,64 @@
         <v>6</v>
       </c>
       <c r="B10" s="74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="111" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E10" s="74">
+        <v>1182</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H10" s="111">
+        <v>1</v>
+      </c>
+      <c r="P10" s="74" t="s">
+        <v>1178</v>
+      </c>
+      <c r="Q10" s="111">
+        <v>30</v>
+      </c>
+      <c r="U10" s="111">
+        <v>1</v>
+      </c>
+      <c r="V10" s="111">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="111">
         <v>2</v>
-      </c>
-      <c r="Q10" s="111">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576 V5:V6 V9:V1048576" xr:uid="{EF7F557D-6948-4EE3-8C24-F51DE661B351}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V6 V10:V1048576 O5:O1048576" xr:uid="{EF7F557D-6948-4EE3-8C24-F51DE661B351}">
       <formula1>external_file_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U6 H5:H6 U10:U1048576 H8:H1048576 N5:N1048576" xr:uid="{7437AD16-BB1D-42F3-A647-3DB0BC5BF784}">
+      <formula1>Dataset_group_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S6 S10:S1048576" xr:uid="{87469BBC-41D2-412B-9F79-50B0C10F8004}">
+      <formula1>equilibrium_constant_determination_method</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Z6 Y8:Z1048576 W5:W1048576" xr:uid="{8E5DCD0E-3113-4254-B04E-6A1A19769DC7}">
+      <formula1>FRET_analysis_ID</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1048576" xr:uid="{58258037-DB7E-441C-95C4-EE25B582EA63}">
       <formula1>relaxation_time_unit</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1048576 N5:N1048576 U5:U6 U9:U1048576" xr:uid="{7437AD16-BB1D-42F3-A647-3DB0BC5BF784}">
-      <formula1>Dataset_group_id</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:F1048576" xr:uid="{9BA7C6E9-6D99-4A36-B409-2D6C7F49D9C3}">
       <formula1>State_id</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1048576" xr:uid="{2CFF6FD5-BDBA-4F14-9AE7-8272BD0D7B91}">
       <formula1>relaxation_time_assignment_choice</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S6 S9:S1048576" xr:uid="{87469BBC-41D2-412B-9F79-50B0C10F8004}">
-      <formula1>equilibrium_constant_determination_method</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y7:Z7 Y6:Z6 Y9:Z1048576 W8 Z8 W9:W1048576 W7 W5 Y5:Z5" xr:uid="{8E5DCD0E-3113-4254-B04E-6A1A19769DC7}">
-      <formula1>FRET_analysis_ID</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5798,7 +5902,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5926,11 +6030,11 @@
       <c r="D5" s="86" t="s">
         <v>965</v>
       </c>
-      <c r="E5" s="86">
-        <v>1</v>
+      <c r="E5" s="86" t="s">
+        <v>1171</v>
       </c>
       <c r="F5" s="86" t="s">
-        <v>908</v>
+        <v>1171</v>
       </c>
       <c r="G5" s="86">
         <v>1</v>
@@ -5961,11 +6065,11 @@
       <c r="D6" s="86" t="s">
         <v>965</v>
       </c>
-      <c r="E6" s="86">
-        <v>1</v>
-      </c>
-      <c r="F6" s="86" t="s">
-        <v>908</v>
+      <c r="E6" s="111" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F6" s="111" t="s">
+        <v>1171</v>
       </c>
       <c r="G6" s="86">
         <v>1</v>
@@ -5996,11 +6100,11 @@
       <c r="D7" s="86" t="s">
         <v>965</v>
       </c>
-      <c r="E7" s="86">
-        <v>1</v>
-      </c>
-      <c r="F7" s="86" t="s">
-        <v>908</v>
+      <c r="E7" s="111" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F7" s="111" t="s">
+        <v>1171</v>
       </c>
       <c r="G7" s="86">
         <v>1</v>
@@ -6031,11 +6135,11 @@
       <c r="D8" s="86" t="s">
         <v>965</v>
       </c>
-      <c r="E8" s="86">
-        <v>1</v>
-      </c>
-      <c r="F8" s="86" t="s">
-        <v>908</v>
+      <c r="E8" s="111" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F8" s="111" t="s">
+        <v>1171</v>
       </c>
       <c r="G8" s="86">
         <v>1</v>
@@ -6066,11 +6170,11 @@
       <c r="D9" s="86" t="s">
         <v>965</v>
       </c>
-      <c r="E9" s="86">
-        <v>1</v>
-      </c>
-      <c r="F9" s="86" t="s">
-        <v>908</v>
+      <c r="E9" s="111" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F9" s="111" t="s">
+        <v>1171</v>
       </c>
       <c r="G9" s="86">
         <v>1</v>
@@ -6101,11 +6205,11 @@
       <c r="D10" s="86" t="s">
         <v>971</v>
       </c>
-      <c r="E10" s="86">
-        <v>2</v>
+      <c r="E10" s="86" t="s">
+        <v>1172</v>
       </c>
       <c r="F10" s="86" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="G10" s="86">
         <v>1</v>
@@ -6136,11 +6240,11 @@
       <c r="D11" s="86" t="s">
         <v>971</v>
       </c>
-      <c r="E11" s="86">
-        <v>2</v>
+      <c r="E11" s="86" t="s">
+        <v>1172</v>
       </c>
       <c r="F11" s="86" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="G11" s="86">
         <v>1</v>
@@ -6171,11 +6275,11 @@
       <c r="D12" s="86" t="s">
         <v>971</v>
       </c>
-      <c r="E12" s="86">
-        <v>2</v>
+      <c r="E12" s="86" t="s">
+        <v>1172</v>
       </c>
       <c r="F12" s="86" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="G12" s="86">
         <v>1</v>
@@ -6206,11 +6310,11 @@
       <c r="D13" s="86" t="s">
         <v>971</v>
       </c>
-      <c r="E13" s="86">
-        <v>2</v>
+      <c r="E13" s="86" t="s">
+        <v>1172</v>
       </c>
       <c r="F13" s="86" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="G13" s="86">
         <v>1</v>
@@ -6241,11 +6345,11 @@
       <c r="D14" s="86" t="s">
         <v>971</v>
       </c>
-      <c r="E14" s="86">
-        <v>2</v>
+      <c r="E14" s="86" t="s">
+        <v>1172</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>954</v>
+        <v>1172</v>
       </c>
       <c r="G14" s="86">
         <v>1</v>
@@ -6299,7 +6403,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6419,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>972</v>
+        <v>1184</v>
       </c>
       <c r="C5" s="88">
         <v>1</v>
@@ -6447,7 +6551,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>973</v>
+        <v>1185</v>
       </c>
       <c r="C6" s="88">
         <v>1</v>
@@ -6496,8 +6600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:BV82"/>
   <sheetViews>
-    <sheetView topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BC4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6697,34 +6801,34 @@
         <v>191</v>
       </c>
       <c r="AJ3" s="77" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AK3" s="31" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AL3" s="31" t="s">
         <v>1007</v>
       </c>
-      <c r="AK3" s="31" t="s">
+      <c r="AM3" s="31" t="s">
         <v>1008</v>
       </c>
-      <c r="AL3" s="31" t="s">
+      <c r="AN3" s="77" t="s">
         <v>1009</v>
       </c>
-      <c r="AM3" s="31" t="s">
+      <c r="AO3" s="31" t="s">
         <v>1010</v>
       </c>
-      <c r="AN3" s="77" t="s">
+      <c r="AP3" s="31" t="s">
         <v>1011</v>
       </c>
-      <c r="AO3" s="31" t="s">
+      <c r="AQ3" s="31" t="s">
         <v>1012</v>
-      </c>
-      <c r="AP3" s="31" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AQ3" s="31" t="s">
-        <v>1014</v>
       </c>
       <c r="AR3" s="77" t="s">
         <v>192</v>
       </c>
       <c r="AS3" s="31" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="AT3" s="31" t="s">
         <v>193</v>
@@ -6748,7 +6852,7 @@
         <v>199</v>
       </c>
       <c r="BA3" s="31" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="BB3" s="31" t="s">
         <v>200</v>
@@ -6921,34 +7025,34 @@
         <v>860</v>
       </c>
       <c r="AJ4" s="72" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AL4" s="13" t="s">
         <v>1015</v>
       </c>
-      <c r="AK4" s="13" t="s">
+      <c r="AM4" s="13" t="s">
         <v>1016</v>
       </c>
-      <c r="AL4" s="13" t="s">
+      <c r="AN4" s="72" t="s">
         <v>1017</v>
       </c>
-      <c r="AM4" s="13" t="s">
+      <c r="AO4" s="13" t="s">
         <v>1018</v>
       </c>
-      <c r="AN4" s="72" t="s">
+      <c r="AP4" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="AO4" s="13" t="s">
+      <c r="AQ4" s="13" t="s">
         <v>1020</v>
-      </c>
-      <c r="AP4" s="13" t="s">
-        <v>1021</v>
-      </c>
-      <c r="AQ4" s="13" t="s">
-        <v>1022</v>
       </c>
       <c r="AR4" s="14" t="s">
         <v>861</v>
       </c>
       <c r="AS4" s="72" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="AT4" s="13" t="s">
         <v>862</v>
@@ -6972,7 +7076,7 @@
         <v>868</v>
       </c>
       <c r="BA4" s="72" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="BB4" s="13" t="s">
         <v>869</v>
@@ -7043,13 +7147,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E5" s="12">
         <v>2</v>
@@ -7058,7 +7162,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="H5" s="18">
         <v>1</v>
@@ -7067,50 +7171,50 @@
         <v>142</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="K5" s="56"/>
       <c r="L5" s="106" t="s">
+        <v>974</v>
+      </c>
+      <c r="M5" s="107" t="s">
+        <v>975</v>
+      </c>
+      <c r="N5" s="107" t="s">
         <v>976</v>
-      </c>
-      <c r="M5" s="107" t="s">
-        <v>977</v>
-      </c>
-      <c r="N5" s="107" t="s">
-        <v>978</v>
       </c>
       <c r="O5" s="107"/>
       <c r="P5" s="107"/>
       <c r="Q5" s="107"/>
       <c r="R5" s="115" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="S5" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="T5" s="107"/>
       <c r="U5" s="107"/>
       <c r="V5" s="97"/>
       <c r="W5" s="97"/>
       <c r="X5" s="106" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="Y5" s="97" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="Z5" s="107"/>
       <c r="AA5" s="107" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="AB5" s="107"/>
       <c r="AC5" s="97"/>
       <c r="AD5" s="107"/>
       <c r="AE5" s="107"/>
       <c r="AF5" s="106" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="AG5" s="107" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="AH5" s="107"/>
       <c r="AI5" s="97"/>
@@ -7127,10 +7231,10 @@
         <v>3</v>
       </c>
       <c r="AU5" s="107" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AV5" s="107" t="s">
         <v>1045</v>
-      </c>
-      <c r="AV5" s="107" t="s">
-        <v>1047</v>
       </c>
       <c r="AW5" s="107" t="s">
         <v>921</v>
@@ -7139,7 +7243,7 @@
         <v>966</v>
       </c>
       <c r="AY5" s="107" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="107"/>
@@ -7150,14 +7254,14 @@
       <c r="BF5" s="5"/>
       <c r="BG5" s="5"/>
       <c r="BH5" s="58" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="BI5" s="5"/>
       <c r="BJ5" s="74" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="BK5" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="BL5" s="107"/>
       <c r="BM5" s="5"/>
@@ -7170,10 +7274,10 @@
       <c r="BR5" s="5"/>
       <c r="BS5" s="5"/>
       <c r="BT5" s="18" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="BU5" s="43" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:74" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -9694,9 +9798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:DW204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9763,7 +9865,7 @@
       <c r="Y1" s="24"/>
       <c r="AG1" s="24"/>
       <c r="AK1" s="76" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="AS1" s="24"/>
       <c r="AT1" s="30"/>
@@ -10066,34 +10168,34 @@
         <v>191</v>
       </c>
       <c r="AK3" s="23" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AL3" s="22" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AM3" s="22" t="s">
         <v>1007</v>
       </c>
-      <c r="AL3" s="22" t="s">
+      <c r="AN3" s="22" t="s">
         <v>1008</v>
       </c>
-      <c r="AM3" s="22" t="s">
+      <c r="AO3" s="22" t="s">
         <v>1009</v>
       </c>
-      <c r="AN3" s="22" t="s">
+      <c r="AP3" s="22" t="s">
         <v>1010</v>
       </c>
-      <c r="AO3" s="22" t="s">
+      <c r="AQ3" s="22" t="s">
         <v>1011</v>
       </c>
-      <c r="AP3" s="22" t="s">
+      <c r="AR3" s="22" t="s">
         <v>1012</v>
-      </c>
-      <c r="AQ3" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AR3" s="22" t="s">
-        <v>1014</v>
       </c>
       <c r="AS3" s="23" t="s">
         <v>192</v>
       </c>
       <c r="AT3" s="22" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="AU3" s="22" t="s">
         <v>193</v>
@@ -10105,7 +10207,7 @@
         <v>195</v>
       </c>
       <c r="AX3" s="22" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="AY3" s="22" t="s">
         <v>197</v>
@@ -10117,7 +10219,7 @@
         <v>199</v>
       </c>
       <c r="BB3" s="22" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="BC3" s="22" t="s">
         <v>200</v>
@@ -10129,7 +10231,7 @@
         <v>202</v>
       </c>
       <c r="BF3" s="22" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="BG3" s="22" t="s">
         <v>204</v>
@@ -10180,7 +10282,7 @@
         <v>219</v>
       </c>
       <c r="BW3" s="28" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="BX3" s="28" t="s">
         <v>901</v>
@@ -10440,34 +10542,34 @@
         <v>277</v>
       </c>
       <c r="AK4" s="72" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AM4" s="13" t="s">
         <v>1024</v>
       </c>
-      <c r="AL4" s="13" t="s">
+      <c r="AN4" s="13" t="s">
         <v>1025</v>
       </c>
-      <c r="AM4" s="13" t="s">
+      <c r="AO4" s="72" t="s">
         <v>1026</v>
       </c>
-      <c r="AN4" s="13" t="s">
+      <c r="AP4" s="13" t="s">
         <v>1027</v>
       </c>
-      <c r="AO4" s="72" t="s">
+      <c r="AQ4" s="13" t="s">
         <v>1028</v>
       </c>
-      <c r="AP4" s="13" t="s">
+      <c r="AR4" s="13" t="s">
         <v>1029</v>
-      </c>
-      <c r="AQ4" s="13" t="s">
-        <v>1030</v>
-      </c>
-      <c r="AR4" s="13" t="s">
-        <v>1031</v>
       </c>
       <c r="AS4" s="14" t="s">
         <v>278</v>
       </c>
       <c r="AT4" s="72" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="AU4" s="13" t="s">
         <v>279</v>
@@ -10491,7 +10593,7 @@
         <v>285</v>
       </c>
       <c r="BB4" s="72" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="BC4" s="13" t="s">
         <v>286</v>
@@ -10554,7 +10656,7 @@
         <v>305</v>
       </c>
       <c r="BW4" s="29" t="s">
-        <v>1161</v>
+        <v>1152</v>
       </c>
       <c r="BX4" s="29" t="s">
         <v>903</v>
@@ -10717,7 +10819,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E5" s="89">
         <v>2</v>
@@ -10726,79 +10828,79 @@
         <v>142</v>
       </c>
       <c r="G5" s="107" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="93" t="s">
+        <v>973</v>
+      </c>
+      <c r="K5" s="94" t="s">
+        <v>984</v>
+      </c>
+      <c r="L5" s="79" t="s">
+        <v>985</v>
+      </c>
+      <c r="M5" s="106" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N5" s="107" t="s">
         <v>975</v>
       </c>
-      <c r="K5" s="94" t="s">
-        <v>986</v>
-      </c>
-      <c r="L5" s="79" t="s">
-        <v>987</v>
-      </c>
-      <c r="M5" s="106" t="s">
-        <v>1055</v>
-      </c>
-      <c r="N5" s="107" t="s">
-        <v>977</v>
-      </c>
       <c r="O5" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="P5" s="107" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Q5" s="107" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="R5" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="S5" s="115" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="T5" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="U5" s="107"/>
       <c r="V5" s="117" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="W5" s="117" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="X5" s="97"/>
       <c r="Y5" s="106" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="Z5" s="97" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="AA5" s="107"/>
       <c r="AB5" s="107"/>
       <c r="AC5" s="107" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="AD5" s="97" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="AE5" s="107"/>
       <c r="AF5" s="107"/>
       <c r="AG5" s="106" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="AH5" s="107" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="AI5" s="96"/>
       <c r="AJ5" s="97"/>
       <c r="AM5" s="107"/>
       <c r="AN5" s="107"/>
       <c r="AO5" s="107" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="AP5" s="50"/>
       <c r="AQ5" s="50"/>
@@ -10813,10 +10915,10 @@
         <v>3</v>
       </c>
       <c r="AV5" s="96" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AW5" s="96" t="s">
         <v>1045</v>
-      </c>
-      <c r="AW5" s="96" t="s">
-        <v>1047</v>
       </c>
       <c r="AX5" s="96" t="s">
         <v>143</v>
@@ -10825,7 +10927,7 @@
         <v>140</v>
       </c>
       <c r="AZ5" s="96" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="BA5" s="96">
         <v>2</v>
@@ -10837,10 +10939,10 @@
         <v>10</v>
       </c>
       <c r="BD5" s="96" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BE5" s="96" t="s">
         <v>1061</v>
-      </c>
-      <c r="BE5" s="96" t="s">
-        <v>1063</v>
       </c>
       <c r="BF5" s="96" t="s">
         <v>966</v>
@@ -10849,26 +10951,26 @@
         <v>921</v>
       </c>
       <c r="BH5" s="96" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="BI5" s="95" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BJ5" s="96" t="s">
         <v>1065</v>
       </c>
-      <c r="BJ5" s="96" t="s">
-        <v>1067</v>
-      </c>
       <c r="BK5" s="74" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="BL5" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="BM5" s="107"/>
       <c r="BN5" s="107" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="BO5" s="117" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="BP5" s="97"/>
       <c r="BQ5" s="107" t="s">
@@ -10889,7 +10991,7 @@
         <v>1</v>
       </c>
       <c r="BX5" s="37" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="BY5" s="99">
         <v>0.35</v>
@@ -10914,20 +11016,20 @@
       <c r="CK5" s="43"/>
       <c r="CL5" s="43"/>
       <c r="CM5" s="101" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="CN5" s="102">
         <v>1.48</v>
       </c>
       <c r="CO5" s="101" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="CP5" s="5"/>
       <c r="CQ5" s="103">
         <v>1</v>
       </c>
-      <c r="CR5" s="104">
-        <v>1</v>
+      <c r="CR5" s="104" t="s">
+        <v>1171</v>
       </c>
       <c r="CS5" s="104">
         <v>53.4</v>
@@ -10942,7 +11044,7 @@
         <v>141</v>
       </c>
       <c r="CW5" s="104">
-        <v>0.78900000000000003</v>
+        <v>0.71</v>
       </c>
       <c r="CX5" s="104">
         <v>1</v>
@@ -11014,7 +11116,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E6" s="89">
         <v>2</v>
@@ -11023,83 +11125,83 @@
         <v>142</v>
       </c>
       <c r="G6" s="107" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="93" t="s">
+        <v>973</v>
+      </c>
+      <c r="K6" s="94" t="s">
+        <v>984</v>
+      </c>
+      <c r="L6" s="79" t="s">
+        <v>985</v>
+      </c>
+      <c r="M6" s="106" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N6" s="107" t="s">
         <v>975</v>
       </c>
-      <c r="K6" s="94" t="s">
-        <v>986</v>
-      </c>
-      <c r="L6" s="79" t="s">
-        <v>987</v>
-      </c>
-      <c r="M6" s="106" t="s">
-        <v>1055</v>
-      </c>
-      <c r="N6" s="107" t="s">
-        <v>977</v>
-      </c>
       <c r="O6" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="P6" s="107" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Q6" s="107" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="R6" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="S6" s="115" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="T6" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="U6" s="107"/>
       <c r="V6" s="117" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="W6" s="117" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="X6" s="97"/>
       <c r="Y6" s="95" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="Z6" s="97" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="AA6" s="96"/>
       <c r="AB6" s="96" t="s">
+        <v>979</v>
+      </c>
+      <c r="AC6" s="96" t="s">
+        <v>980</v>
+      </c>
+      <c r="AD6" s="97" t="s">
         <v>981</v>
-      </c>
-      <c r="AC6" s="96" t="s">
-        <v>982</v>
-      </c>
-      <c r="AD6" s="97" t="s">
-        <v>983</v>
       </c>
       <c r="AE6" s="96"/>
       <c r="AF6" s="96" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="AG6" s="106" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="AH6" s="107" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="AI6" s="96"/>
       <c r="AJ6" s="97"/>
       <c r="AM6" s="107"/>
       <c r="AN6" s="107"/>
       <c r="AO6" s="107" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="AP6" s="50"/>
       <c r="AQ6" s="50"/>
@@ -11114,10 +11216,10 @@
         <v>3</v>
       </c>
       <c r="AV6" s="107" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AW6" s="96" t="s">
         <v>1045</v>
-      </c>
-      <c r="AW6" s="96" t="s">
-        <v>1047</v>
       </c>
       <c r="AX6" s="96" t="s">
         <v>143</v>
@@ -11126,7 +11228,7 @@
         <v>140</v>
       </c>
       <c r="AZ6" s="107" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="BA6" s="96">
         <v>2</v>
@@ -11138,10 +11240,10 @@
         <v>10</v>
       </c>
       <c r="BD6" s="96" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BE6" s="107" t="s">
         <v>1061</v>
-      </c>
-      <c r="BE6" s="107" t="s">
-        <v>1063</v>
       </c>
       <c r="BF6" s="96" t="s">
         <v>966</v>
@@ -11150,26 +11252,26 @@
         <v>921</v>
       </c>
       <c r="BH6" s="107" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="BI6" s="106" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BJ6" s="96" t="s">
         <v>1065</v>
       </c>
-      <c r="BJ6" s="96" t="s">
-        <v>1067</v>
-      </c>
       <c r="BK6" s="74" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="BL6" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="BM6" s="107"/>
       <c r="BN6" s="107" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="BO6" s="117" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="BP6" s="97"/>
       <c r="BQ6" s="107" t="s">
@@ -11190,7 +11292,7 @@
         <v>1</v>
       </c>
       <c r="BX6" s="37" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="BY6" s="99">
         <v>0.35</v>
@@ -11215,20 +11317,20 @@
       <c r="CK6" s="43"/>
       <c r="CL6" s="43"/>
       <c r="CM6" s="101" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="CN6" s="102">
         <v>1.48</v>
       </c>
       <c r="CO6" s="101" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="CP6" s="5"/>
       <c r="CQ6" s="103">
         <v>2</v>
       </c>
-      <c r="CR6" s="104">
-        <v>2</v>
+      <c r="CR6" s="104" t="s">
+        <v>1172</v>
       </c>
       <c r="CS6" s="104">
         <v>60.2</v>
@@ -11243,7 +11345,7 @@
         <v>141</v>
       </c>
       <c r="CW6" s="104">
-        <v>0.109</v>
+        <v>0.19</v>
       </c>
       <c r="CX6" s="104">
         <v>1</v>
@@ -11315,7 +11417,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -11324,83 +11426,83 @@
         <v>142</v>
       </c>
       <c r="G7" s="107" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="97" t="s">
+        <v>973</v>
+      </c>
+      <c r="K7" s="97" t="s">
+        <v>984</v>
+      </c>
+      <c r="L7" s="79" t="s">
+        <v>985</v>
+      </c>
+      <c r="M7" s="106" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N7" s="107" t="s">
         <v>975</v>
       </c>
-      <c r="K7" s="97" t="s">
-        <v>986</v>
-      </c>
-      <c r="L7" s="79" t="s">
-        <v>987</v>
-      </c>
-      <c r="M7" s="106" t="s">
-        <v>1055</v>
-      </c>
-      <c r="N7" s="107" t="s">
-        <v>977</v>
-      </c>
       <c r="O7" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="P7" s="107" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Q7" s="107" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="R7" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="S7" s="115" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="T7" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="U7" s="107"/>
       <c r="V7" s="117" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="W7" s="117" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="X7" s="97"/>
       <c r="Y7" s="106" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="Z7" s="97" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="AA7" s="107"/>
       <c r="AB7" s="107" t="s">
+        <v>979</v>
+      </c>
+      <c r="AC7" s="107" t="s">
+        <v>980</v>
+      </c>
+      <c r="AD7" s="97" t="s">
         <v>981</v>
-      </c>
-      <c r="AC7" s="107" t="s">
-        <v>982</v>
-      </c>
-      <c r="AD7" s="97" t="s">
-        <v>983</v>
       </c>
       <c r="AE7" s="107"/>
       <c r="AF7" s="107" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="AG7" s="106" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="AH7" s="107" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="AI7" s="107"/>
       <c r="AJ7" s="97"/>
       <c r="AM7" s="107"/>
       <c r="AN7" s="107"/>
       <c r="AO7" s="107" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="AP7" s="50"/>
       <c r="AQ7" s="50"/>
@@ -11415,10 +11517,10 @@
         <v>3</v>
       </c>
       <c r="AV7" s="107" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AW7" s="107" t="s">
         <v>1045</v>
-      </c>
-      <c r="AW7" s="107" t="s">
-        <v>1047</v>
       </c>
       <c r="AX7" s="107" t="s">
         <v>143</v>
@@ -11427,7 +11529,7 @@
         <v>140</v>
       </c>
       <c r="AZ7" s="107" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="BA7" s="107">
         <v>2</v>
@@ -11439,10 +11541,10 @@
         <v>3</v>
       </c>
       <c r="BD7" s="107" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BE7" s="107" t="s">
         <v>1061</v>
-      </c>
-      <c r="BE7" s="107" t="s">
-        <v>1063</v>
       </c>
       <c r="BF7" s="107" t="s">
         <v>966</v>
@@ -11451,26 +11553,26 @@
         <v>921</v>
       </c>
       <c r="BH7" s="107" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="BI7" s="106" t="s">
+        <v>1064</v>
+      </c>
+      <c r="BJ7" s="107" t="s">
         <v>1066</v>
       </c>
-      <c r="BJ7" s="107" t="s">
-        <v>1068</v>
-      </c>
       <c r="BK7" s="74" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="BL7" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="BM7" s="107"/>
       <c r="BN7" s="107" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="BO7" s="117" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="BP7" s="97"/>
       <c r="BQ7" s="107" t="s">
@@ -11491,7 +11593,7 @@
         <v>2</v>
       </c>
       <c r="BX7" s="37" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="BY7" s="4"/>
       <c r="BZ7" s="5"/>
@@ -11502,10 +11604,10 @@
       <c r="CE7" s="5"/>
       <c r="CF7" s="5"/>
       <c r="CG7" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="CH7" s="43" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="CI7" s="43"/>
       <c r="CJ7" s="43">
@@ -11516,20 +11618,20 @@
       </c>
       <c r="CL7" s="43"/>
       <c r="CM7" s="4" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="CN7" s="61">
         <v>1.0900000000000001</v>
       </c>
       <c r="CO7" s="67" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="CP7" s="5"/>
       <c r="CQ7" s="4">
         <v>3</v>
       </c>
-      <c r="CR7" s="5">
-        <v>1</v>
+      <c r="CR7" s="5" t="s">
+        <v>1171</v>
       </c>
       <c r="CS7" s="5">
         <v>50.2</v>
@@ -11544,7 +11646,7 @@
         <v>144</v>
       </c>
       <c r="CW7" s="5">
-        <v>0.78900000000000003</v>
+        <v>0.71</v>
       </c>
       <c r="CX7" s="5">
         <v>1</v>
@@ -11607,7 +11709,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E8" s="106">
         <v>2</v>
@@ -11616,76 +11718,76 @@
         <v>142</v>
       </c>
       <c r="G8" s="107" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="H8" s="107"/>
       <c r="I8" s="107"/>
       <c r="J8" s="97" t="s">
+        <v>973</v>
+      </c>
+      <c r="K8" s="97" t="s">
+        <v>984</v>
+      </c>
+      <c r="L8" s="79" t="s">
+        <v>985</v>
+      </c>
+      <c r="M8" s="106" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N8" s="107" t="s">
         <v>975</v>
       </c>
-      <c r="K8" s="97" t="s">
-        <v>986</v>
-      </c>
-      <c r="L8" s="79" t="s">
-        <v>987</v>
-      </c>
-      <c r="M8" s="106" t="s">
-        <v>1055</v>
-      </c>
-      <c r="N8" s="107" t="s">
-        <v>977</v>
-      </c>
       <c r="O8" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="P8" s="107" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="Q8" s="107" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="R8" s="107" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="S8" s="115" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="T8" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="U8" s="107"/>
       <c r="V8" s="117" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="W8" s="117" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="X8" s="97"/>
       <c r="Y8" s="106" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="Z8" s="97" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="AA8" s="107"/>
       <c r="AB8" s="107" t="s">
+        <v>979</v>
+      </c>
+      <c r="AC8" s="107" t="s">
+        <v>980</v>
+      </c>
+      <c r="AD8" s="97" t="s">
         <v>981</v>
-      </c>
-      <c r="AC8" s="107" t="s">
-        <v>982</v>
-      </c>
-      <c r="AD8" s="97" t="s">
-        <v>983</v>
       </c>
       <c r="AE8" s="107"/>
       <c r="AF8" s="107" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="AG8" s="106" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="AH8" s="107" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="AI8" s="107"/>
       <c r="AJ8" s="97"/>
@@ -11694,7 +11796,7 @@
       <c r="AM8" s="107"/>
       <c r="AN8" s="107"/>
       <c r="AO8" s="107" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="AP8" s="50"/>
       <c r="AQ8" s="50"/>
@@ -11709,10 +11811,10 @@
         <v>3</v>
       </c>
       <c r="AV8" s="107" t="s">
+        <v>1043</v>
+      </c>
+      <c r="AW8" s="107" t="s">
         <v>1045</v>
-      </c>
-      <c r="AW8" s="107" t="s">
-        <v>1047</v>
       </c>
       <c r="AX8" s="107" t="s">
         <v>143</v>
@@ -11721,7 +11823,7 @@
         <v>140</v>
       </c>
       <c r="AZ8" s="107" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="BA8" s="107">
         <v>2</v>
@@ -11733,10 +11835,10 @@
         <v>3</v>
       </c>
       <c r="BD8" s="107" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BE8" s="107" t="s">
         <v>1061</v>
-      </c>
-      <c r="BE8" s="107" t="s">
-        <v>1063</v>
       </c>
       <c r="BF8" s="107" t="s">
         <v>966</v>
@@ -11745,26 +11847,26 @@
         <v>921</v>
       </c>
       <c r="BH8" s="107" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="BI8" s="106" t="s">
+        <v>1064</v>
+      </c>
+      <c r="BJ8" s="107" t="s">
         <v>1066</v>
       </c>
-      <c r="BJ8" s="107" t="s">
-        <v>1068</v>
-      </c>
       <c r="BK8" s="74" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="BL8" s="116" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="BM8" s="107"/>
       <c r="BN8" s="107" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="BO8" s="117" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="BP8" s="97"/>
       <c r="BQ8" s="107" t="s">
@@ -11785,7 +11887,7 @@
         <v>2</v>
       </c>
       <c r="BX8" s="37" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="BY8" s="106"/>
       <c r="BZ8" s="107"/>
@@ -11796,10 +11898,10 @@
       <c r="CE8" s="107"/>
       <c r="CF8" s="107"/>
       <c r="CG8" s="42" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="CH8" s="78" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="CI8" s="78"/>
       <c r="CJ8" s="78">
@@ -11810,20 +11912,20 @@
       </c>
       <c r="CL8" s="78"/>
       <c r="CM8" s="106" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="CN8" s="61">
         <v>1.0900000000000001</v>
       </c>
       <c r="CO8" s="106" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="CP8" s="107"/>
       <c r="CQ8" s="106">
         <v>4</v>
       </c>
-      <c r="CR8" s="107">
-        <v>2</v>
+      <c r="CR8" s="107" t="s">
+        <v>1172</v>
       </c>
       <c r="CS8" s="107">
         <v>58.7</v>
@@ -11838,7 +11940,7 @@
         <v>144</v>
       </c>
       <c r="CW8" s="107">
-        <v>0.109</v>
+        <v>0.19</v>
       </c>
       <c r="CX8" s="107">
         <v>1</v>
@@ -34753,7 +34855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -34965,7 +35069,7 @@
         <v>10</v>
       </c>
       <c r="R5" s="108" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="S5" s="108">
         <v>100</v>
@@ -35033,7 +35137,7 @@
         <v>10</v>
       </c>
       <c r="R6" s="109" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="S6" s="109">
         <v>100</v>
@@ -35082,7 +35186,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B1" s="111"/>
     </row>
@@ -35091,7 +35195,7 @@
         <v>641</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -35102,10 +35206,10 @@
     </row>
     <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -35113,7 +35217,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -35125,7 +35229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -36006,7 +36112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -36029,10 +36135,10 @@
         <v>377</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1179</v>
+        <v>1170</v>
       </c>
       <c r="L1" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
       <c r="N1" t="s">
         <v>383</v>
@@ -36041,14 +36147,14 @@
         <v>527</v>
       </c>
       <c r="S1" s="111" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="T1" s="111"/>
       <c r="U1" s="111" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
       <c r="W1" s="111" t="s">
-        <v>1165</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -36077,14 +36183,14 @@
         <v>7</v>
       </c>
       <c r="S2" s="111" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
       <c r="T2" s="111"/>
       <c r="U2" s="111" t="s">
-        <v>1168</v>
+        <v>1159</v>
       </c>
       <c r="W2" s="131" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -36113,14 +36219,14 @@
         <v>519</v>
       </c>
       <c r="S3" s="111" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
       <c r="T3" s="111"/>
       <c r="U3" s="111" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="W3" s="131" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -36146,11 +36252,11 @@
         <v>520</v>
       </c>
       <c r="S4" s="111" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
       <c r="T4" s="111"/>
       <c r="W4" s="131" t="s">
-        <v>1159</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -36277,7 +36383,7 @@
         <v>85</v>
       </c>
       <c r="K12" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
       <c r="L12" t="s">
         <v>56</v>
@@ -36503,8 +36609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36554,7 +36660,7 @@
         <v>656</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>657</v>
@@ -36642,7 +36748,7 @@
         <v>336</v>
       </c>
       <c r="H4" s="70" t="s">
-        <v>1177</v>
+        <v>1168</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>337</v>
@@ -36684,17 +36790,17 @@
         <v>920</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H5" s="66"/>
       <c r="I5" s="65" t="s">
         <v>95</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="K5" s="111" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -36717,17 +36823,17 @@
         <v>920</v>
       </c>
       <c r="G6" s="66" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="H6" s="66"/>
       <c r="I6" s="111" t="s">
         <v>95</v>
       </c>
       <c r="J6" s="111" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="K6" s="111" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -36915,8 +37021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -37226,7 +37332,7 @@
   <dimension ref="A1:H202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -37966,7 +38072,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
+      <selection activeCell="A4" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -38004,7 +38110,8 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>491</v>
       </c>
@@ -38015,7 +38122,7 @@
         <v>493</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>494</v>
@@ -38176,8 +38283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -38253,7 +38360,7 @@
         <v>674</v>
       </c>
       <c r="T2" s="75" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -38315,7 +38422,7 @@
         <v>107</v>
       </c>
       <c r="T3" s="87" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -38385,7 +38492,7 @@
         <v>381</v>
       </c>
       <c r="T4" s="70" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
@@ -38411,10 +38518,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="65" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="J5" s="65">
         <v>1</v>
@@ -38430,7 +38537,7 @@
       </c>
       <c r="N5" s="65"/>
       <c r="O5" s="65" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="P5" s="65" t="s">
         <v>953</v>
@@ -38468,10 +38575,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="111" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="J6" s="65">
         <v>1</v>
@@ -38487,7 +38594,7 @@
       </c>
       <c r="N6" s="65"/>
       <c r="O6" s="65" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="P6" s="65" t="s">
         <v>953</v>
@@ -38572,7 +38679,7 @@
       <c r="B13" s="65"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="7">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"comparative model, experimental model, integrative model, ab initio model, other"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update number of connections in multi_state_scheme example
Update number of connections in multi_state_scheme for example to now include 2 relaxation times and 4 kinetic rates
</commit_message>
<xml_diff>
--- a/example/xls_example.xlsx
+++ b/example/xls_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\flr2mmcif_devel\20240426_modification_of_example\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\flr2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D4213-D746-41C4-8BD6-9C2A54BD8AC8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102ABE5-DC7A-4620-8397-8B2689CEA728}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1190">
   <si>
     <t>Model number</t>
   </si>
@@ -3617,9 +3617,6 @@
     <t>tr2 - second relaxation time for the system</t>
   </si>
   <si>
-    <t>tr3 - third relaxation time for the system</t>
-  </si>
-  <si>
     <t>k12 - Kinetic transition rate constant for connection betwen C1 and C2</t>
   </si>
   <si>
@@ -3654,6 +3651,12 @@
   </si>
   <si>
     <t>k32</t>
+  </si>
+  <si>
+    <t>k21</t>
+  </si>
+  <si>
+    <t>k21 - Kinetic transition rate constant for connection betwen C2 and C1</t>
   </si>
 </sst>
 </file>
@@ -4573,7 +4576,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5335,10 +5338,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3412B954-CC29-49CA-9B82-95A52B6CE843}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5617,10 +5620,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="111" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D5" s="111" t="s">
         <v>1180</v>
-      </c>
-      <c r="D5" s="111" t="s">
-        <v>1181</v>
       </c>
       <c r="E5" s="130" t="s">
         <v>1171</v>
@@ -5664,16 +5667,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="111" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D6" s="111" t="s">
         <v>1180</v>
-      </c>
-      <c r="D6" s="111" t="s">
-        <v>1181</v>
       </c>
       <c r="E6" s="74" t="s">
         <v>1172</v>
       </c>
       <c r="F6" s="111" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="H6" s="111">
         <v>1</v>
@@ -5709,81 +5712,42 @@
         <v>1</v>
       </c>
       <c r="C7" s="111" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D7" s="111" t="s">
         <v>1180</v>
       </c>
-      <c r="D7" s="111" t="s">
-        <v>1181</v>
-      </c>
       <c r="E7" s="74" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F7" s="111" t="s">
         <v>1173</v>
-      </c>
-      <c r="F7" s="111" t="s">
-        <v>1172</v>
       </c>
       <c r="H7" s="111">
         <v>1</v>
       </c>
-      <c r="I7" s="74" t="s">
-        <v>1176</v>
-      </c>
-      <c r="J7" s="81" t="s">
-        <v>1160</v>
-      </c>
-      <c r="K7" s="111">
-        <v>10</v>
-      </c>
-      <c r="L7" s="111" t="s">
-        <v>1147</v>
-      </c>
-      <c r="N7" s="111">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="111">
+        <v>4</v>
+      </c>
+      <c r="B8" s="74">
         <v>1</v>
       </c>
-      <c r="O7" s="111">
-        <v>1</v>
-      </c>
-      <c r="W7" s="74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
-        <v>4</v>
-      </c>
-      <c r="B8" s="74">
-        <v>2</v>
-      </c>
       <c r="C8" s="111" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>1183</v>
+        <v>1179</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>1180</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>1171</v>
-      </c>
-      <c r="F8" s="45" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F8" s="111" t="s">
         <v>1172</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>1186</v>
       </c>
       <c r="H8" s="111">
         <v>1</v>
-      </c>
-      <c r="P8" s="74" t="s">
-        <v>1177</v>
-      </c>
-      <c r="Q8" s="111">
-        <v>20</v>
-      </c>
-      <c r="U8" s="111">
-        <v>1</v>
-      </c>
-      <c r="V8" s="111">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="111">
-        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -5794,28 +5758,28 @@
         <v>2</v>
       </c>
       <c r="C9" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D9" s="45" t="s">
         <v>1182</v>
       </c>
-      <c r="D9" s="45" t="s">
-        <v>1183</v>
-      </c>
       <c r="E9" s="74" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F9" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="F9" s="45" t="s">
-        <v>1173</v>
-      </c>
       <c r="G9" s="45" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="H9" s="111">
         <v>1</v>
       </c>
       <c r="P9" s="74" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="Q9" s="111">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="U9" s="111">
         <v>1</v>
@@ -5835,16 +5799,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>1182</v>
       </c>
-      <c r="D10" s="45" t="s">
-        <v>1183</v>
-      </c>
       <c r="E10" s="74" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>1188</v>
@@ -5853,10 +5817,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="74" t="s">
-        <v>1178</v>
+        <v>1189</v>
       </c>
       <c r="Q10" s="111">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="U10" s="111">
         <v>1</v>
@@ -5868,18 +5832,100 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="45">
+        <v>7</v>
+      </c>
+      <c r="B11" s="74">
+        <v>2</v>
+      </c>
+      <c r="C11" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E11" s="74" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H11" s="111">
+        <v>1</v>
+      </c>
+      <c r="P11" s="74" t="s">
+        <v>1178</v>
+      </c>
+      <c r="Q11" s="111">
+        <v>150</v>
+      </c>
+      <c r="U11" s="111">
+        <v>1</v>
+      </c>
+      <c r="V11" s="111">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="45">
+        <v>8</v>
+      </c>
+      <c r="B12" s="74">
+        <v>2</v>
+      </c>
+      <c r="C12" s="111" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E12" s="74" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H12" s="111">
+        <v>1</v>
+      </c>
+      <c r="P12" s="74" t="s">
+        <v>1177</v>
+      </c>
+      <c r="Q12" s="111">
+        <v>30</v>
+      </c>
+      <c r="U12" s="111">
+        <v>1</v>
+      </c>
+      <c r="V12" s="111">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="111">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V6 V10:V1048576 O5:O1048576" xr:uid="{EF7F557D-6948-4EE3-8C24-F51DE661B351}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V6 V12:V1048576 O5:O1048576" xr:uid="{EF7F557D-6948-4EE3-8C24-F51DE661B351}">
       <formula1>external_file_id</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U6 H5:H6 U10:U1048576 H8:H1048576 N5:N1048576" xr:uid="{7437AD16-BB1D-42F3-A647-3DB0BC5BF784}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U6 H5:H6 U12:U1048576 N5:N1048576 H9:H1048576" xr:uid="{7437AD16-BB1D-42F3-A647-3DB0BC5BF784}">
       <formula1>Dataset_group_id</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S6 S10:S1048576" xr:uid="{87469BBC-41D2-412B-9F79-50B0C10F8004}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S6 S12:S1048576" xr:uid="{87469BBC-41D2-412B-9F79-50B0C10F8004}">
       <formula1>equilibrium_constant_determination_method</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Z6 Y8:Z1048576 W5:W1048576" xr:uid="{8E5DCD0E-3113-4254-B04E-6A1A19769DC7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Z6 W5:W1048576 Y9:Z1048576" xr:uid="{8E5DCD0E-3113-4254-B04E-6A1A19769DC7}">
       <formula1>FRET_analysis_ID</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1048576" xr:uid="{58258037-DB7E-441C-95C4-EE25B582EA63}">
@@ -6523,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C5" s="88">
         <v>1</v>
@@ -6551,7 +6597,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C6" s="88">
         <v>1</v>

</xml_diff>

<commit_message>
Match IHMCIF w.r.t. use of collection of models
Adapt the template and the script to use "Collection of models" instead of "Ensemble" in IHMCIF. The internal usage was not modified yet.
</commit_message>
<xml_diff>
--- a/example/xls_example.xlsx
+++ b/example/xls_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\flr2mmcif\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\flr2mmcif_development\20240619_update_excel_sheet\flr2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102ABE5-DC7A-4620-8397-8B2689CEA728}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEA03A9-E4BA-43DD-AABE-1A9E3F4971D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Multi-state modeling" sheetId="7" r:id="rId12"/>
     <sheet name="Multi-state scheme" sheetId="22" r:id="rId13"/>
     <sheet name="Models" sheetId="2" r:id="rId14"/>
-    <sheet name="Ensemble Info" sheetId="17" r:id="rId15"/>
+    <sheet name="Collection of models" sheetId="17" r:id="rId15"/>
     <sheet name="Reference_measurements" sheetId="20" r:id="rId16"/>
     <sheet name="FLR" sheetId="8" r:id="rId17"/>
     <sheet name="FLR_FPS_MPP_group" sheetId="18" r:id="rId18"/>
@@ -2144,9 +2144,6 @@
     <t>Time-ordered modeling?</t>
   </si>
   <si>
-    <t>Ensemble?</t>
-  </si>
-  <si>
     <t>The ID of the software used (Tab 'Software') in this step of the modeling protocol.</t>
   </si>
   <si>
@@ -2204,33 +2201,12 @@
     <t>The name of the model group.</t>
   </si>
   <si>
-    <t>Is the model a representative of an ensemble?</t>
-  </si>
-  <si>
     <t>If it is a representative, what was the selection criterion?</t>
   </si>
   <si>
-    <t>The name of the ensemble</t>
-  </si>
-  <si>
-    <t>How was the ensemble clustered (the method)? Please choose one.</t>
-  </si>
-  <si>
     <t>What was the feature for clustering?</t>
   </si>
   <si>
-    <t>How many models are in the ensemble? (This might be more than the number of models deposited, if e.g. only representatives are deposited)</t>
-  </si>
-  <si>
-    <t>How many models from the ensemble are deposited?</t>
-  </si>
-  <si>
-    <t>What is the precision value of the ensemble?</t>
-  </si>
-  <si>
-    <t>The File ID of the ensemble (Tab 'External_files')</t>
-  </si>
-  <si>
     <t>Most of these entries correspond to the global parameters in the FPS program.</t>
   </si>
   <si>
@@ -2405,12 +2381,6 @@
     <t>The ID of the modeling protocol (Tab 'Modeling protocol').</t>
   </si>
   <si>
-    <t>Description of an ensemble of structural models.</t>
-  </si>
-  <si>
-    <t>The post process ID by which the ensemble was created (Tab 'Modeling_post_process').</t>
-  </si>
-  <si>
     <t>The ID of the model group (Tab 'Models').</t>
   </si>
   <si>
@@ -3587,9 +3557,6 @@
     <t>Ensemble FRET data</t>
   </si>
   <si>
-    <t>Template version 1.7</t>
-  </si>
-  <si>
     <t>Details to the entity</t>
   </si>
   <si>
@@ -3638,12 +3605,6 @@
     <t>Transition rate constants between states</t>
   </si>
   <si>
-    <t>Ensemble for C1</t>
-  </si>
-  <si>
-    <t>Ensemble for C2</t>
-  </si>
-  <si>
     <t>k12</t>
   </si>
   <si>
@@ -3657,6 +3618,45 @@
   </si>
   <si>
     <t>k21 - Kinetic transition rate constant for connection betwen C2 and C1</t>
+  </si>
+  <si>
+    <t>Template version 1.8</t>
+  </si>
+  <si>
+    <t>Collection of models?</t>
+  </si>
+  <si>
+    <t>Is the model a representative of a collection of models?</t>
+  </si>
+  <si>
+    <t>Model collection for C1</t>
+  </si>
+  <si>
+    <t>Model collection for C2</t>
+  </si>
+  <si>
+    <t>Description of a collection of structural models.</t>
+  </si>
+  <si>
+    <t>The name of the collection of models</t>
+  </si>
+  <si>
+    <t>The post process ID by which the collection of models was created (Tab 'Modeling_post_process').</t>
+  </si>
+  <si>
+    <t>How was the collection of models clustered (the method)? Please choose one.</t>
+  </si>
+  <si>
+    <t>How many models are in the collection? (This might be more than the number of models deposited, if e.g. only representatives are deposited)</t>
+  </si>
+  <si>
+    <t>How many models from the collection are deposited?</t>
+  </si>
+  <si>
+    <t>What is the precision value of the collection of models?</t>
+  </si>
+  <si>
+    <t>The File ID of the collection of models (Tab 'External_files')</t>
   </si>
 </sst>
 </file>
@@ -4576,19 +4576,19 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1166</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>799</v>
+        <v>789</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>794</v>
+        <v>784</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4612,7 +4612,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>798</v>
+        <v>788</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4620,7 +4620,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4628,7 +4628,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>800</v>
+        <v>790</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4652,7 +4652,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -4665,7 +4665,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4676,7 +4676,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="20" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
@@ -4690,10 +4690,10 @@
         <v>675</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>677</v>
@@ -4720,10 +4720,10 @@
         <v>684</v>
       </c>
       <c r="N2" s="20" t="s">
+        <v>1178</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>685</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -4837,10 +4837,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>955</v>
+        <v>945</v>
       </c>
       <c r="G5" s="83" t="s">
-        <v>956</v>
+        <v>946</v>
       </c>
       <c r="H5" s="83"/>
       <c r="I5" s="83">
@@ -4853,13 +4853,13 @@
         <v>143</v>
       </c>
       <c r="L5" s="83" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="N5" s="83" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="O5" s="83">
         <v>1</v>
@@ -4882,10 +4882,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="83" t="s">
-        <v>955</v>
+        <v>945</v>
       </c>
       <c r="G6" s="83" t="s">
-        <v>959</v>
+        <v>949</v>
       </c>
       <c r="H6" s="83"/>
       <c r="I6" s="83">
@@ -4898,13 +4898,13 @@
         <v>143</v>
       </c>
       <c r="L6" s="83" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="M6" s="83" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="N6" s="83" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="O6" s="83">
         <v>1</v>
@@ -4944,7 +4944,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="20" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
@@ -4952,37 +4952,37 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>688</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>760</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>754</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>689</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>761</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>762</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>690</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>691</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>692</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>693</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="20" t="s">
         <v>694</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -5081,13 +5081,13 @@
         <v>1</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="H5" s="84" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="I5" s="84" t="s">
-        <v>962</v>
+        <v>952</v>
       </c>
       <c r="J5" s="84"/>
       <c r="K5" s="84"/>
@@ -5140,7 +5140,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="20" customFormat="1" ht="63" x14ac:dyDescent="0.25">
@@ -5148,31 +5148,31 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>696</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>697</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>764</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>698</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>699</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
+        <v>895</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>757</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>700</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>905</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>765</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -5198,7 +5198,7 @@
         <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>906</v>
+        <v>896</v>
       </c>
       <c r="I3" t="s">
         <v>135</v>
@@ -5230,7 +5230,7 @@
         <v>418</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>907</v>
+        <v>897</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>419</v>
@@ -5244,7 +5244,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="C5" s="85">
         <v>1</v>
@@ -5256,16 +5256,16 @@
         <v>0.05</v>
       </c>
       <c r="F5" s="85" t="s">
-        <v>963</v>
+        <v>953</v>
       </c>
       <c r="G5" s="85" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="I5" s="85">
         <v>1</v>
       </c>
       <c r="J5" s="85" t="s">
-        <v>964</v>
+        <v>954</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5273,7 +5273,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="C6" s="85">
         <v>2</v>
@@ -5285,16 +5285,16 @@
         <v>0.05</v>
       </c>
       <c r="F6" s="85" t="s">
-        <v>963</v>
+        <v>953</v>
       </c>
       <c r="G6" s="85" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="I6" s="85">
         <v>2</v>
       </c>
       <c r="J6" s="85" t="s">
-        <v>964</v>
+        <v>954</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5302,7 +5302,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -5314,13 +5314,13 @@
         <v>0.05</v>
       </c>
       <c r="F7" s="111" t="s">
-        <v>963</v>
+        <v>953</v>
       </c>
       <c r="G7" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="J7" t="s">
-        <v>964</v>
+        <v>954</v>
       </c>
     </row>
   </sheetData>
@@ -5370,7 +5370,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
       <c r="B1" s="111"/>
       <c r="E1" s="111"/>
@@ -5385,79 +5385,79 @@
         <v>641</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>1146</v>
+        <v>1136</v>
       </c>
       <c r="C2" s="119" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D2" s="120" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E2" s="118" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F2" s="119" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G2" s="119" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H2" s="120" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I2" s="118" t="s">
+        <v>1076</v>
+      </c>
+      <c r="J2" s="119" t="s">
+        <v>1143</v>
+      </c>
+      <c r="K2" s="119" t="s">
+        <v>1077</v>
+      </c>
+      <c r="L2" s="119" t="s">
+        <v>1078</v>
+      </c>
+      <c r="M2" s="119" t="s">
+        <v>1079</v>
+      </c>
+      <c r="N2" s="119" t="s">
         <v>1080</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="O2" s="120" t="s">
         <v>1081</v>
       </c>
-      <c r="E2" s="118" t="s">
+      <c r="P2" s="118" t="s">
         <v>1082</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="Q2" s="121" t="s">
         <v>1083</v>
       </c>
-      <c r="G2" s="119" t="s">
+      <c r="R2" s="121" t="s">
         <v>1084</v>
       </c>
-      <c r="H2" s="120" t="s">
+      <c r="S2" s="119" t="s">
         <v>1085</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="T2" s="119" t="s">
         <v>1086</v>
       </c>
-      <c r="J2" s="119" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K2" s="119" t="s">
+      <c r="U2" s="121" t="s">
         <v>1087</v>
       </c>
-      <c r="L2" s="119" t="s">
+      <c r="V2" s="119" t="s">
         <v>1088</v>
       </c>
-      <c r="M2" s="119" t="s">
+      <c r="W2" s="118" t="s">
         <v>1089</v>
       </c>
-      <c r="N2" s="119" t="s">
+      <c r="X2" s="119" t="s">
+        <v>1151</v>
+      </c>
+      <c r="Y2" s="119" t="s">
         <v>1090</v>
       </c>
-      <c r="O2" s="120" t="s">
-        <v>1091</v>
-      </c>
-      <c r="P2" s="118" t="s">
-        <v>1092</v>
-      </c>
-      <c r="Q2" s="121" t="s">
-        <v>1093</v>
-      </c>
-      <c r="R2" s="121" t="s">
-        <v>1094</v>
-      </c>
-      <c r="S2" s="119" t="s">
-        <v>1095</v>
-      </c>
-      <c r="T2" s="119" t="s">
-        <v>1096</v>
-      </c>
-      <c r="U2" s="121" t="s">
-        <v>1097</v>
-      </c>
-      <c r="V2" s="119" t="s">
-        <v>1098</v>
-      </c>
-      <c r="W2" s="118" t="s">
-        <v>1099</v>
-      </c>
-      <c r="X2" s="119" t="s">
-        <v>1161</v>
-      </c>
-      <c r="Y2" s="119" t="s">
-        <v>1100</v>
-      </c>
       <c r="Z2" s="120" t="s">
-        <v>1162</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -5465,151 +5465,151 @@
         <v>129</v>
       </c>
       <c r="B3" s="122" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D3" s="123" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E3" s="124" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G3" s="81" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H3" s="123" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I3" s="122" t="s">
+        <v>1097</v>
+      </c>
+      <c r="K3" s="81" t="s">
+        <v>1098</v>
+      </c>
+      <c r="L3" s="81" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M3" s="81" t="s">
+        <v>1100</v>
+      </c>
+      <c r="N3" s="81" t="s">
         <v>1101</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="O3" s="123" t="s">
         <v>1102</v>
       </c>
-      <c r="D3" s="123" t="s">
+      <c r="P3" s="122" t="s">
         <v>1103</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="Q3" s="81" t="s">
         <v>1104</v>
       </c>
-      <c r="F3" s="81" t="s">
-        <v>1104</v>
-      </c>
-      <c r="G3" s="81" t="s">
+      <c r="R3" s="81" t="s">
         <v>1105</v>
       </c>
-      <c r="H3" s="123" t="s">
+      <c r="S3" s="81" t="s">
         <v>1106</v>
       </c>
-      <c r="I3" s="122" t="s">
+      <c r="T3" s="81" t="s">
         <v>1107</v>
       </c>
-      <c r="K3" s="81" t="s">
+      <c r="U3" s="81" t="s">
         <v>1108</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="V3" s="81" t="s">
         <v>1109</v>
       </c>
-      <c r="M3" s="81" t="s">
+      <c r="W3" s="122" t="s">
         <v>1110</v>
       </c>
-      <c r="N3" s="81" t="s">
+      <c r="Y3" s="81" t="s">
         <v>1111</v>
-      </c>
-      <c r="O3" s="123" t="s">
-        <v>1112</v>
-      </c>
-      <c r="P3" s="122" t="s">
-        <v>1113</v>
-      </c>
-      <c r="Q3" s="81" t="s">
-        <v>1114</v>
-      </c>
-      <c r="R3" s="81" t="s">
-        <v>1115</v>
-      </c>
-      <c r="S3" s="81" t="s">
-        <v>1116</v>
-      </c>
-      <c r="T3" s="81" t="s">
-        <v>1117</v>
-      </c>
-      <c r="U3" s="81" t="s">
-        <v>1118</v>
-      </c>
-      <c r="V3" s="81" t="s">
-        <v>1119</v>
-      </c>
-      <c r="W3" s="122" t="s">
-        <v>1120</v>
-      </c>
-      <c r="Y3" s="81" t="s">
-        <v>1121</v>
       </c>
       <c r="Z3" s="123"/>
     </row>
     <row r="4" spans="1:26" s="70" customFormat="1" ht="48" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D4" s="126" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E4" s="127" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H4" s="126" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I4" s="125" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>1144</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>1121</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>1122</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="M4" s="16" t="s">
         <v>1123</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="N4" s="16" t="s">
         <v>1124</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="O4" s="126" t="s">
         <v>1125</v>
       </c>
-      <c r="E4" s="127" t="s">
+      <c r="P4" s="125" t="s">
         <v>1126</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
         <v>1127</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>1128</v>
       </c>
-      <c r="H4" s="126" t="s">
+      <c r="S4" s="16" t="s">
         <v>1129</v>
       </c>
-      <c r="I4" s="125" t="s">
+      <c r="T4" s="16" t="s">
         <v>1130</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="U4" s="16" t="s">
+        <v>1131</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>1132</v>
+      </c>
+      <c r="W4" s="125" t="s">
+        <v>1133</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>1153</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Z4" s="126" t="s">
         <v>1154</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>1131</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>1132</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>1133</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>1134</v>
-      </c>
-      <c r="O4" s="126" t="s">
-        <v>1135</v>
-      </c>
-      <c r="P4" s="125" t="s">
-        <v>1136</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>1137</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>1138</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>1139</v>
-      </c>
-      <c r="T4" s="16" t="s">
-        <v>1140</v>
-      </c>
-      <c r="U4" s="16" t="s">
-        <v>1141</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>1142</v>
-      </c>
-      <c r="W4" s="125" t="s">
-        <v>1143</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>1163</v>
-      </c>
-      <c r="Y4" s="16" t="s">
-        <v>1144</v>
-      </c>
-      <c r="Z4" s="126" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -5620,31 +5620,31 @@
         <v>1</v>
       </c>
       <c r="C5" s="111" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="D5" s="111" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
       <c r="E5" s="130" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F5" s="111" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="H5" s="111">
         <v>1</v>
       </c>
       <c r="I5" s="130" t="s">
-        <v>1174</v>
+        <v>1163</v>
       </c>
       <c r="J5" s="81" t="s">
-        <v>1160</v>
+        <v>1150</v>
       </c>
       <c r="K5" s="45">
         <v>120</v>
       </c>
       <c r="L5" s="111" t="s">
-        <v>1147</v>
+        <v>1137</v>
       </c>
       <c r="N5" s="111">
         <v>1</v>
@@ -5667,31 +5667,31 @@
         <v>1</v>
       </c>
       <c r="C6" s="111" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="D6" s="111" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F6" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="H6" s="111">
         <v>1</v>
       </c>
       <c r="I6" s="74" t="s">
-        <v>1175</v>
+        <v>1164</v>
       </c>
       <c r="J6" s="81" t="s">
-        <v>1160</v>
+        <v>1150</v>
       </c>
       <c r="K6" s="111">
         <v>70</v>
       </c>
       <c r="L6" s="111" t="s">
-        <v>1147</v>
+        <v>1137</v>
       </c>
       <c r="N6" s="111">
         <v>1</v>
@@ -5712,16 +5712,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="111" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="D7" s="111" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
       <c r="E7" s="74" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F7" s="111" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="H7" s="111">
         <v>1</v>
@@ -5735,16 +5735,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="111" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="D8" s="111" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="F8" s="111" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="H8" s="111">
         <v>1</v>
@@ -5758,25 +5758,25 @@
         <v>2</v>
       </c>
       <c r="C9" s="111" t="s">
-        <v>1181</v>
+        <v>1170</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F9" s="45" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G9" s="45" t="s">
         <v>1172</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>1185</v>
       </c>
       <c r="H9" s="111">
         <v>1</v>
       </c>
       <c r="P9" s="74" t="s">
-        <v>1176</v>
+        <v>1165</v>
       </c>
       <c r="Q9" s="111">
         <v>20</v>
@@ -5799,25 +5799,25 @@
         <v>2</v>
       </c>
       <c r="C10" s="111" t="s">
-        <v>1181</v>
+        <v>1170</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
       <c r="E10" s="74" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G10" s="45" t="s">
-        <v>1188</v>
+        <v>1175</v>
       </c>
       <c r="H10" s="111">
         <v>1</v>
       </c>
       <c r="P10" s="74" t="s">
-        <v>1189</v>
+        <v>1176</v>
       </c>
       <c r="Q10" s="111">
         <v>300</v>
@@ -5840,25 +5840,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="111" t="s">
-        <v>1181</v>
+        <v>1170</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
       <c r="E11" s="74" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F11" s="45" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G11" s="45" t="s">
         <v>1173</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>1186</v>
       </c>
       <c r="H11" s="111">
         <v>1</v>
       </c>
       <c r="P11" s="74" t="s">
-        <v>1178</v>
+        <v>1167</v>
       </c>
       <c r="Q11" s="111">
         <v>150</v>
@@ -5881,25 +5881,25 @@
         <v>2</v>
       </c>
       <c r="C12" s="111" t="s">
-        <v>1181</v>
+        <v>1170</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>1187</v>
+        <v>1174</v>
       </c>
       <c r="H12" s="111">
         <v>1</v>
       </c>
       <c r="P12" s="74" t="s">
-        <v>1177</v>
+        <v>1166</v>
       </c>
       <c r="Q12" s="111">
         <v>30</v>
@@ -5948,14 +5948,14 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="20" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
@@ -5963,34 +5963,34 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>702</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>703</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
+        <v>759</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>760</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>761</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>762</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>763</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>1179</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>704</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>767</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>768</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>769</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>770</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>771</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>705</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -6074,13 +6074,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="E5" s="86" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F5" s="86" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G5" s="86">
         <v>1</v>
@@ -6092,7 +6092,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="86" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="K5" s="86" t="s">
         <v>7</v>
@@ -6103,19 +6103,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="86" t="s">
-        <v>967</v>
+        <v>957</v>
       </c>
       <c r="C6" s="86">
         <v>1</v>
       </c>
       <c r="D6" s="86" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="E6" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F6" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G6" s="86">
         <v>1</v>
@@ -6127,7 +6127,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K6" s="86" t="s">
         <v>128</v>
@@ -6138,19 +6138,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="86" t="s">
-        <v>968</v>
+        <v>958</v>
       </c>
       <c r="C7" s="86">
         <v>1</v>
       </c>
       <c r="D7" s="86" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="E7" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F7" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G7" s="86">
         <v>1</v>
@@ -6162,7 +6162,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K7" s="86" t="s">
         <v>128</v>
@@ -6173,19 +6173,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="86" t="s">
-        <v>969</v>
+        <v>959</v>
       </c>
       <c r="C8" s="86">
         <v>1</v>
       </c>
       <c r="D8" s="86" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="E8" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F8" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G8" s="86">
         <v>1</v>
@@ -6197,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K8" s="86" t="s">
         <v>128</v>
@@ -6208,19 +6208,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="86" t="s">
-        <v>970</v>
+        <v>960</v>
       </c>
       <c r="C9" s="86">
         <v>1</v>
       </c>
       <c r="D9" s="86" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="E9" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="F9" s="111" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="G9" s="86">
         <v>1</v>
@@ -6232,7 +6232,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K9" s="86" t="s">
         <v>128</v>
@@ -6249,13 +6249,13 @@
         <v>2</v>
       </c>
       <c r="D10" s="86" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="E10" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F10" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G10" s="86">
         <v>1</v>
@@ -6267,7 +6267,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="86" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="K10" s="86" t="s">
         <v>7</v>
@@ -6278,19 +6278,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="86" t="s">
-        <v>967</v>
+        <v>957</v>
       </c>
       <c r="C11" s="86">
         <v>2</v>
       </c>
       <c r="D11" s="86" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="E11" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F11" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G11" s="86">
         <v>1</v>
@@ -6302,7 +6302,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K11" s="86" t="s">
         <v>128</v>
@@ -6313,19 +6313,19 @@
         <v>8</v>
       </c>
       <c r="B12" s="86" t="s">
-        <v>968</v>
+        <v>958</v>
       </c>
       <c r="C12" s="86">
         <v>2</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F12" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G12" s="86">
         <v>1</v>
@@ -6337,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K12" s="86" t="s">
         <v>128</v>
@@ -6348,19 +6348,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="86" t="s">
-        <v>969</v>
+        <v>959</v>
       </c>
       <c r="C13" s="86">
         <v>2</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F13" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G13" s="86">
         <v>1</v>
@@ -6372,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K13" s="86" t="s">
         <v>128</v>
@@ -6383,19 +6383,19 @@
         <v>10</v>
       </c>
       <c r="B14" s="86" t="s">
-        <v>970</v>
+        <v>960</v>
       </c>
       <c r="C14" s="86">
         <v>2</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="E14" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="G14" s="86">
         <v>1</v>
@@ -6407,7 +6407,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="86" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="K14" s="86" t="s">
         <v>128</v>
@@ -6449,7 +6449,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6465,7 +6465,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>772</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="20" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -6473,31 +6473,31 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>707</v>
+        <v>1183</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>773</v>
+        <v>1184</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>708</v>
+        <v>1185</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>710</v>
+        <v>1186</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>711</v>
+        <v>1187</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>712</v>
+        <v>1188</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>713</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="110.25" hidden="1" x14ac:dyDescent="0.25">
@@ -6569,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="C5" s="88">
         <v>1</v>
@@ -6581,7 +6581,7 @@
         <v>56</v>
       </c>
       <c r="F5" s="88" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="G5" s="88">
         <v>5</v>
@@ -6597,7 +6597,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="C6" s="88">
         <v>1</v>
@@ -6609,7 +6609,7 @@
         <v>56</v>
       </c>
       <c r="F6" s="88" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="G6" s="88">
         <v>5</v>
@@ -6685,7 +6685,7 @@
   <sheetData>
     <row r="1" spans="1:74" s="113" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="113" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="F1" s="114"/>
       <c r="H1" s="114"/>
@@ -6698,12 +6698,12 @@
       <c r="BH1" s="114"/>
       <c r="BJ1" s="114"/>
       <c r="BT1" s="114" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
     </row>
     <row r="2" spans="1:74" s="16" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>148</v>
@@ -6745,28 +6745,28 @@
         <v>641</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>893</v>
+        <v>883</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="E3" s="77" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="F3" s="77" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="H3" s="77" t="s">
         <v>165</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>166</v>
@@ -6847,34 +6847,34 @@
         <v>191</v>
       </c>
       <c r="AJ3" s="77" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="AK3" s="31" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="AL3" s="31" t="s">
-        <v>1007</v>
+        <v>997</v>
       </c>
       <c r="AM3" s="31" t="s">
-        <v>1008</v>
+        <v>998</v>
       </c>
       <c r="AN3" s="77" t="s">
-        <v>1009</v>
+        <v>999</v>
       </c>
       <c r="AO3" s="31" t="s">
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="AP3" s="31" t="s">
-        <v>1011</v>
+        <v>1001</v>
       </c>
       <c r="AQ3" s="31" t="s">
-        <v>1012</v>
+        <v>1002</v>
       </c>
       <c r="AR3" s="77" t="s">
         <v>192</v>
       </c>
       <c r="AS3" s="31" t="s">
-        <v>1070</v>
+        <v>1060</v>
       </c>
       <c r="AT3" s="31" t="s">
         <v>193</v>
@@ -6898,7 +6898,7 @@
         <v>199</v>
       </c>
       <c r="BA3" s="31" t="s">
-        <v>1072</v>
+        <v>1062</v>
       </c>
       <c r="BB3" s="31" t="s">
         <v>200</v>
@@ -6955,237 +6955,237 @@
         <v>217</v>
       </c>
       <c r="BT3" s="77" t="s">
-        <v>889</v>
+        <v>879</v>
       </c>
       <c r="BU3" s="31" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="BV3" s="31" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
     </row>
     <row r="4" spans="1:74" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>819</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>884</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>817</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>818</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>892</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>816</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>838</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>822</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>823</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>824</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>825</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>826</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>827</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>828</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>829</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>894</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>827</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>828</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>902</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>826</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="P4" s="13" t="s">
+        <v>830</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>832</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>833</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>834</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>835</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>836</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>837</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>839</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>840</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>841</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>842</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>843</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>844</v>
+      </c>
+      <c r="AD4" s="13" t="s">
+        <v>845</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>846</v>
+      </c>
+      <c r="AF4" s="14" t="s">
+        <v>847</v>
+      </c>
+      <c r="AG4" s="13" t="s">
         <v>848</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>832</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>833</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>834</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>835</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>836</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>837</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>838</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>839</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>840</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>841</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>842</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>843</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>844</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>845</v>
-      </c>
-      <c r="V4" s="13" t="s">
-        <v>846</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>847</v>
-      </c>
-      <c r="X4" s="14" t="s">
+      <c r="AH4" s="13" t="s">
         <v>849</v>
       </c>
-      <c r="Y4" s="13" t="s">
+      <c r="AI4" s="13" t="s">
         <v>850</v>
       </c>
-      <c r="Z4" s="13" t="s">
+      <c r="AJ4" s="72" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>1004</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AM4" s="13" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AN4" s="72" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AO4" s="13" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AQ4" s="13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="AR4" s="14" t="s">
         <v>851</v>
       </c>
-      <c r="AA4" s="13" t="s">
+      <c r="AS4" s="72" t="s">
+        <v>1061</v>
+      </c>
+      <c r="AT4" s="13" t="s">
         <v>852</v>
       </c>
-      <c r="AB4" s="13" t="s">
+      <c r="AU4" s="13" t="s">
         <v>853</v>
       </c>
-      <c r="AC4" s="13" t="s">
+      <c r="AV4" s="13" t="s">
         <v>854</v>
       </c>
-      <c r="AD4" s="13" t="s">
+      <c r="AW4" s="13" t="s">
         <v>855</v>
       </c>
-      <c r="AE4" s="13" t="s">
+      <c r="AX4" s="13" t="s">
         <v>856</v>
       </c>
-      <c r="AF4" s="14" t="s">
+      <c r="AY4" s="13" t="s">
         <v>857</v>
       </c>
-      <c r="AG4" s="13" t="s">
+      <c r="AZ4" s="13" t="s">
         <v>858</v>
       </c>
-      <c r="AH4" s="13" t="s">
+      <c r="BA4" s="72" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BB4" s="13" t="s">
         <v>859</v>
       </c>
-      <c r="AI4" s="13" t="s">
+      <c r="BC4" s="13" t="s">
         <v>860</v>
       </c>
-      <c r="AJ4" s="72" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AK4" s="13" t="s">
-        <v>1014</v>
-      </c>
-      <c r="AL4" s="13" t="s">
-        <v>1015</v>
-      </c>
-      <c r="AM4" s="13" t="s">
-        <v>1016</v>
-      </c>
-      <c r="AN4" s="72" t="s">
-        <v>1017</v>
-      </c>
-      <c r="AO4" s="13" t="s">
-        <v>1018</v>
-      </c>
-      <c r="AP4" s="13" t="s">
-        <v>1019</v>
-      </c>
-      <c r="AQ4" s="13" t="s">
-        <v>1020</v>
-      </c>
-      <c r="AR4" s="14" t="s">
+      <c r="BD4" s="13" t="s">
         <v>861</v>
       </c>
-      <c r="AS4" s="72" t="s">
-        <v>1071</v>
-      </c>
-      <c r="AT4" s="13" t="s">
+      <c r="BE4" s="13" t="s">
         <v>862</v>
       </c>
-      <c r="AU4" s="13" t="s">
+      <c r="BF4" s="13" t="s">
         <v>863</v>
       </c>
-      <c r="AV4" s="13" t="s">
+      <c r="BG4" s="13" t="s">
         <v>864</v>
       </c>
-      <c r="AW4" s="13" t="s">
+      <c r="BH4" s="72" t="s">
         <v>865</v>
       </c>
-      <c r="AX4" s="13" t="s">
+      <c r="BI4" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="AY4" s="13" t="s">
+      <c r="BJ4" s="14" t="s">
         <v>867</v>
       </c>
-      <c r="AZ4" s="13" t="s">
+      <c r="BK4" s="13" t="s">
         <v>868</v>
       </c>
-      <c r="BA4" s="72" t="s">
-        <v>1073</v>
-      </c>
-      <c r="BB4" s="13" t="s">
+      <c r="BL4" s="13" t="s">
         <v>869</v>
       </c>
-      <c r="BC4" s="13" t="s">
+      <c r="BM4" s="13" t="s">
         <v>870</v>
       </c>
-      <c r="BD4" s="13" t="s">
+      <c r="BN4" s="13" t="s">
         <v>871</v>
       </c>
-      <c r="BE4" s="13" t="s">
+      <c r="BO4" s="13" t="s">
         <v>872</v>
       </c>
-      <c r="BF4" s="13" t="s">
+      <c r="BP4" s="13" t="s">
         <v>873</v>
       </c>
-      <c r="BG4" s="13" t="s">
+      <c r="BQ4" s="13" t="s">
         <v>874</v>
       </c>
-      <c r="BH4" s="72" t="s">
+      <c r="BR4" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="BI4" s="13" t="s">
+      <c r="BS4" s="13" t="s">
         <v>876</v>
       </c>
-      <c r="BJ4" s="14" t="s">
+      <c r="BT4" s="14" t="s">
         <v>877</v>
       </c>
-      <c r="BK4" s="13" t="s">
+      <c r="BU4" s="14" t="s">
         <v>878</v>
       </c>
-      <c r="BL4" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="BM4" s="13" t="s">
-        <v>880</v>
-      </c>
-      <c r="BN4" s="13" t="s">
-        <v>881</v>
-      </c>
-      <c r="BO4" s="13" t="s">
+      <c r="BV4" s="13" t="s">
         <v>882</v>
-      </c>
-      <c r="BP4" s="13" t="s">
-        <v>883</v>
-      </c>
-      <c r="BQ4" s="13" t="s">
-        <v>884</v>
-      </c>
-      <c r="BR4" s="13" t="s">
-        <v>885</v>
-      </c>
-      <c r="BS4" s="13" t="s">
-        <v>886</v>
-      </c>
-      <c r="BT4" s="14" t="s">
-        <v>887</v>
-      </c>
-      <c r="BU4" s="14" t="s">
-        <v>888</v>
-      </c>
-      <c r="BV4" s="13" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="5" spans="1:74" ht="63" x14ac:dyDescent="0.25">
@@ -7193,13 +7193,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>996</v>
+        <v>986</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>997</v>
+        <v>987</v>
       </c>
       <c r="E5" s="12">
         <v>2</v>
@@ -7208,7 +7208,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>998</v>
+        <v>988</v>
       </c>
       <c r="H5" s="18">
         <v>1</v>
@@ -7217,50 +7217,50 @@
         <v>142</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>1049</v>
+        <v>1039</v>
       </c>
       <c r="K5" s="56"/>
       <c r="L5" s="106" t="s">
-        <v>974</v>
+        <v>964</v>
       </c>
       <c r="M5" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="N5" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="O5" s="107"/>
       <c r="P5" s="107"/>
       <c r="Q5" s="107"/>
       <c r="R5" s="115" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="S5" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="T5" s="107"/>
       <c r="U5" s="107"/>
       <c r="V5" s="97"/>
       <c r="W5" s="97"/>
       <c r="X5" s="106" t="s">
-        <v>1041</v>
+        <v>1031</v>
       </c>
       <c r="Y5" s="97" t="s">
-        <v>1042</v>
+        <v>1032</v>
       </c>
       <c r="Z5" s="107"/>
       <c r="AA5" s="107" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AB5" s="107"/>
       <c r="AC5" s="97"/>
       <c r="AD5" s="107"/>
       <c r="AE5" s="107"/>
       <c r="AF5" s="106" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AG5" s="107" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="AH5" s="107"/>
       <c r="AI5" s="97"/>
@@ -7277,19 +7277,19 @@
         <v>3</v>
       </c>
       <c r="AU5" s="107" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AV5" s="107" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="AW5" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="AX5" s="107" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="AY5" s="107" t="s">
-        <v>1046</v>
+        <v>1036</v>
       </c>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="107"/>
@@ -7300,30 +7300,30 @@
       <c r="BF5" s="5"/>
       <c r="BG5" s="5"/>
       <c r="BH5" s="58" t="s">
-        <v>1050</v>
+        <v>1040</v>
       </c>
       <c r="BI5" s="5"/>
       <c r="BJ5" s="74" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="BK5" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="BL5" s="107"/>
       <c r="BM5" s="5"/>
       <c r="BN5" s="6"/>
       <c r="BO5" s="6"/>
       <c r="BP5" s="5" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BQ5" s="5"/>
       <c r="BR5" s="5"/>
       <c r="BS5" s="5"/>
       <c r="BT5" s="18" t="s">
-        <v>999</v>
+        <v>989</v>
       </c>
       <c r="BU5" s="43" t="s">
-        <v>1000</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" spans="1:74" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -9901,7 +9901,7 @@
   <sheetData>
     <row r="1" spans="1:127" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
       <c r="B1" s="24"/>
       <c r="E1" s="24"/>
@@ -9911,7 +9911,7 @@
       <c r="Y1" s="24"/>
       <c r="AG1" s="24"/>
       <c r="AK1" s="76" t="s">
-        <v>1021</v>
+        <v>1011</v>
       </c>
       <c r="AS1" s="24"/>
       <c r="AT1" s="30"/>
@@ -9921,10 +9921,10 @@
       <c r="BW1" s="26"/>
       <c r="BX1" s="26"/>
       <c r="BY1" s="24" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="CG1" s="38" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
       <c r="CH1" s="39"/>
       <c r="CI1" s="39"/>
@@ -9940,7 +9940,7 @@
     </row>
     <row r="2" spans="1:127" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>147</v>
@@ -10043,7 +10043,7 @@
       <c r="BV2" s="16"/>
       <c r="BW2" s="27"/>
       <c r="BX2" s="27" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="BY2" s="17" t="s">
         <v>160</v>
@@ -10056,13 +10056,13 @@
       <c r="CE2" s="16"/>
       <c r="CF2" s="16"/>
       <c r="CG2" s="17" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="CH2" s="16"/>
       <c r="CI2" s="16"/>
       <c r="CJ2" s="16"/>
       <c r="CK2" s="16" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="CL2" s="35"/>
       <c r="CM2" s="16" t="s">
@@ -10112,16 +10112,16 @@
         <v>636</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>165</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="G3" s="54" t="s">
         <v>166</v>
@@ -10133,13 +10133,13 @@
         <v>167</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="M3" s="23" t="s">
         <v>168</v>
@@ -10214,46 +10214,46 @@
         <v>191</v>
       </c>
       <c r="AK3" s="23" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="AL3" s="22" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="AM3" s="22" t="s">
-        <v>1007</v>
+        <v>997</v>
       </c>
       <c r="AN3" s="22" t="s">
-        <v>1008</v>
+        <v>998</v>
       </c>
       <c r="AO3" s="22" t="s">
-        <v>1009</v>
+        <v>999</v>
       </c>
       <c r="AP3" s="22" t="s">
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="AQ3" s="22" t="s">
-        <v>1011</v>
+        <v>1001</v>
       </c>
       <c r="AR3" s="22" t="s">
-        <v>1012</v>
+        <v>1002</v>
       </c>
       <c r="AS3" s="23" t="s">
         <v>192</v>
       </c>
       <c r="AT3" s="22" t="s">
-        <v>1074</v>
+        <v>1064</v>
       </c>
       <c r="AU3" s="22" t="s">
         <v>193</v>
       </c>
       <c r="AV3" s="22" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="AW3" s="22" t="s">
         <v>195</v>
       </c>
       <c r="AX3" s="22" t="s">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="AY3" s="22" t="s">
         <v>197</v>
@@ -10265,19 +10265,19 @@
         <v>199</v>
       </c>
       <c r="BB3" s="22" t="s">
-        <v>1076</v>
+        <v>1066</v>
       </c>
       <c r="BC3" s="22" t="s">
         <v>200</v>
       </c>
       <c r="BD3" s="22" t="s">
-        <v>911</v>
+        <v>901</v>
       </c>
       <c r="BE3" s="22" t="s">
         <v>202</v>
       </c>
       <c r="BF3" s="22" t="s">
-        <v>1031</v>
+        <v>1021</v>
       </c>
       <c r="BG3" s="22" t="s">
         <v>204</v>
@@ -10328,47 +10328,47 @@
         <v>219</v>
       </c>
       <c r="BW3" s="28" t="s">
-        <v>1145</v>
+        <v>1135</v>
       </c>
       <c r="BX3" s="28" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="BY3" s="23" t="s">
         <v>220</v>
       </c>
       <c r="BZ3" s="22" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="CA3" s="22"/>
       <c r="CB3" s="22" t="s">
-        <v>804</v>
+        <v>794</v>
       </c>
       <c r="CC3" s="22" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="CD3" s="22" t="s">
-        <v>806</v>
+        <v>796</v>
       </c>
       <c r="CE3" s="22" t="s">
         <v>221</v>
       </c>
       <c r="CF3" s="22" t="s">
+        <v>797</v>
+      </c>
+      <c r="CG3" s="23" t="s">
+        <v>806</v>
+      </c>
+      <c r="CH3" s="22" t="s">
         <v>807</v>
       </c>
-      <c r="CG3" s="23" t="s">
-        <v>816</v>
-      </c>
-      <c r="CH3" s="22" t="s">
-        <v>817</v>
-      </c>
       <c r="CI3" s="22" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="CJ3" s="22" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="CK3" s="22" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c r="CL3" s="41"/>
       <c r="CM3" s="22" t="s">
@@ -10510,10 +10510,10 @@
         <v>253</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>254</v>
@@ -10588,34 +10588,34 @@
         <v>277</v>
       </c>
       <c r="AK4" s="72" t="s">
-        <v>1022</v>
+        <v>1012</v>
       </c>
       <c r="AL4" s="13" t="s">
-        <v>1023</v>
+        <v>1013</v>
       </c>
       <c r="AM4" s="13" t="s">
-        <v>1024</v>
+        <v>1014</v>
       </c>
       <c r="AN4" s="13" t="s">
-        <v>1025</v>
+        <v>1015</v>
       </c>
       <c r="AO4" s="72" t="s">
-        <v>1026</v>
+        <v>1016</v>
       </c>
       <c r="AP4" s="13" t="s">
-        <v>1027</v>
+        <v>1017</v>
       </c>
       <c r="AQ4" s="13" t="s">
-        <v>1028</v>
+        <v>1018</v>
       </c>
       <c r="AR4" s="13" t="s">
-        <v>1029</v>
+        <v>1019</v>
       </c>
       <c r="AS4" s="14" t="s">
         <v>278</v>
       </c>
       <c r="AT4" s="72" t="s">
-        <v>1075</v>
+        <v>1065</v>
       </c>
       <c r="AU4" s="13" t="s">
         <v>279</v>
@@ -10639,7 +10639,7 @@
         <v>285</v>
       </c>
       <c r="BB4" s="72" t="s">
-        <v>1077</v>
+        <v>1067</v>
       </c>
       <c r="BC4" s="13" t="s">
         <v>286</v>
@@ -10702,10 +10702,10 @@
         <v>305</v>
       </c>
       <c r="BW4" s="29" t="s">
-        <v>1152</v>
+        <v>1142</v>
       </c>
       <c r="BX4" s="29" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="BY4" s="14" t="s">
         <v>306</v>
@@ -10732,19 +10732,19 @@
         <v>313</v>
       </c>
       <c r="CG4" s="14" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="CH4" s="13" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="CI4" s="13" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="CJ4" s="13" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="CK4" s="13" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="CL4" s="34"/>
       <c r="CM4" s="13" t="s">
@@ -10760,37 +10760,37 @@
         <v>317</v>
       </c>
       <c r="CQ4" s="14" t="s">
+        <v>769</v>
+      </c>
+      <c r="CR4" s="13" t="s">
+        <v>770</v>
+      </c>
+      <c r="CS4" s="13" t="s">
+        <v>771</v>
+      </c>
+      <c r="CT4" s="13" t="s">
+        <v>772</v>
+      </c>
+      <c r="CU4" s="13" t="s">
+        <v>773</v>
+      </c>
+      <c r="CV4" s="13" t="s">
+        <v>774</v>
+      </c>
+      <c r="CW4" s="13" t="s">
+        <v>775</v>
+      </c>
+      <c r="CX4" s="13" t="s">
+        <v>776</v>
+      </c>
+      <c r="CY4" s="13" t="s">
+        <v>777</v>
+      </c>
+      <c r="CZ4" s="13" t="s">
+        <v>778</v>
+      </c>
+      <c r="DA4" s="7" t="s">
         <v>779</v>
-      </c>
-      <c r="CR4" s="13" t="s">
-        <v>780</v>
-      </c>
-      <c r="CS4" s="13" t="s">
-        <v>781</v>
-      </c>
-      <c r="CT4" s="13" t="s">
-        <v>782</v>
-      </c>
-      <c r="CU4" s="13" t="s">
-        <v>783</v>
-      </c>
-      <c r="CV4" s="13" t="s">
-        <v>784</v>
-      </c>
-      <c r="CW4" s="13" t="s">
-        <v>785</v>
-      </c>
-      <c r="CX4" s="13" t="s">
-        <v>786</v>
-      </c>
-      <c r="CY4" s="13" t="s">
-        <v>787</v>
-      </c>
-      <c r="CZ4" s="13" t="s">
-        <v>788</v>
-      </c>
-      <c r="DA4" s="7" t="s">
-        <v>789</v>
       </c>
       <c r="DC4" s="14" t="s">
         <v>318</v>
@@ -10865,7 +10865,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="E5" s="89">
         <v>2</v>
@@ -10874,79 +10874,79 @@
         <v>142</v>
       </c>
       <c r="G5" s="107" t="s">
-        <v>1052</v>
+        <v>1042</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="93" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="K5" s="94" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="L5" s="79" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="M5" s="106" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="N5" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="O5" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="P5" s="107" t="s">
-        <v>1054</v>
+        <v>1044</v>
       </c>
       <c r="Q5" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="R5" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="S5" s="115" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="T5" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="U5" s="107"/>
       <c r="V5" s="117" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
       <c r="W5" s="117" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="X5" s="97"/>
       <c r="Y5" s="106" t="s">
-        <v>1041</v>
+        <v>1031</v>
       </c>
       <c r="Z5" s="97" t="s">
-        <v>1042</v>
+        <v>1032</v>
       </c>
       <c r="AA5" s="107"/>
       <c r="AB5" s="107"/>
       <c r="AC5" s="107" t="s">
-        <v>1057</v>
+        <v>1047</v>
       </c>
       <c r="AD5" s="97" t="s">
-        <v>1058</v>
+        <v>1048</v>
       </c>
       <c r="AE5" s="107"/>
       <c r="AF5" s="107"/>
       <c r="AG5" s="106" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AH5" s="107" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="AI5" s="96"/>
       <c r="AJ5" s="97"/>
       <c r="AM5" s="107"/>
       <c r="AN5" s="107"/>
       <c r="AO5" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="AP5" s="50"/>
       <c r="AQ5" s="50"/>
@@ -10955,16 +10955,16 @@
         <v>1</v>
       </c>
       <c r="AT5" s="80" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="AU5" s="96">
         <v>3</v>
       </c>
       <c r="AV5" s="96" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AW5" s="96" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="AX5" s="96" t="s">
         <v>143</v>
@@ -10973,58 +10973,58 @@
         <v>140</v>
       </c>
       <c r="AZ5" s="96" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="BA5" s="96">
         <v>2</v>
       </c>
       <c r="BB5" s="107" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="BC5" s="96">
         <v>10</v>
       </c>
       <c r="BD5" s="96" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="BE5" s="96" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="BF5" s="96" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="BG5" s="96" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BH5" s="96" t="s">
-        <v>1062</v>
+        <v>1052</v>
       </c>
       <c r="BI5" s="95" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="BJ5" s="96" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
       <c r="BK5" s="74" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="BL5" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="BM5" s="107"/>
       <c r="BN5" s="107" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="BO5" s="117" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="BP5" s="97"/>
       <c r="BQ5" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BR5" s="107"/>
       <c r="BS5" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BT5" s="96"/>
       <c r="BU5" s="98">
@@ -11037,7 +11037,7 @@
         <v>1</v>
       </c>
       <c r="BX5" s="37" t="s">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="BY5" s="99">
         <v>0.35</v>
@@ -11062,20 +11062,20 @@
       <c r="CK5" s="43"/>
       <c r="CL5" s="43"/>
       <c r="CM5" s="101" t="s">
-        <v>982</v>
+        <v>972</v>
       </c>
       <c r="CN5" s="102">
         <v>1.48</v>
       </c>
       <c r="CO5" s="101" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="CP5" s="5"/>
       <c r="CQ5" s="103">
         <v>1</v>
       </c>
       <c r="CR5" s="104" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="CS5" s="104">
         <v>53.4</v>
@@ -11162,7 +11162,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="E6" s="89">
         <v>2</v>
@@ -11171,83 +11171,83 @@
         <v>142</v>
       </c>
       <c r="G6" s="107" t="s">
-        <v>1052</v>
+        <v>1042</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="93" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="K6" s="94" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="L6" s="79" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="M6" s="106" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="N6" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="O6" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="P6" s="107" t="s">
-        <v>1054</v>
+        <v>1044</v>
       </c>
       <c r="Q6" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="R6" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="S6" s="115" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="T6" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="U6" s="107"/>
       <c r="V6" s="117" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
       <c r="W6" s="117" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="X6" s="97"/>
       <c r="Y6" s="95" t="s">
-        <v>977</v>
+        <v>967</v>
       </c>
       <c r="Z6" s="97" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="AA6" s="96"/>
       <c r="AB6" s="96" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AC6" s="96" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="AD6" s="97" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="AE6" s="96"/>
       <c r="AF6" s="96" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AG6" s="106" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AH6" s="107" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="AI6" s="96"/>
       <c r="AJ6" s="97"/>
       <c r="AM6" s="107"/>
       <c r="AN6" s="107"/>
       <c r="AO6" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="AP6" s="50"/>
       <c r="AQ6" s="50"/>
@@ -11256,16 +11256,16 @@
         <v>1</v>
       </c>
       <c r="AT6" s="80" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="AU6" s="96">
         <v>3</v>
       </c>
       <c r="AV6" s="107" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AW6" s="96" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="AX6" s="96" t="s">
         <v>143</v>
@@ -11274,58 +11274,58 @@
         <v>140</v>
       </c>
       <c r="AZ6" s="107" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="BA6" s="96">
         <v>2</v>
       </c>
       <c r="BB6" s="107" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="BC6" s="96">
         <v>10</v>
       </c>
       <c r="BD6" s="96" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="BE6" s="107" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="BF6" s="96" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="BG6" s="96" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BH6" s="107" t="s">
-        <v>1062</v>
+        <v>1052</v>
       </c>
       <c r="BI6" s="106" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="BJ6" s="96" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
       <c r="BK6" s="74" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="BL6" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="BM6" s="107"/>
       <c r="BN6" s="107" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="BO6" s="117" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="BP6" s="97"/>
       <c r="BQ6" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BR6" s="107"/>
       <c r="BS6" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BT6" s="96"/>
       <c r="BU6" s="98">
@@ -11338,7 +11338,7 @@
         <v>1</v>
       </c>
       <c r="BX6" s="37" t="s">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="BY6" s="99">
         <v>0.35</v>
@@ -11363,20 +11363,20 @@
       <c r="CK6" s="43"/>
       <c r="CL6" s="43"/>
       <c r="CM6" s="101" t="s">
-        <v>982</v>
+        <v>972</v>
       </c>
       <c r="CN6" s="102">
         <v>1.48</v>
       </c>
       <c r="CO6" s="101" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="CP6" s="5"/>
       <c r="CQ6" s="103">
         <v>2</v>
       </c>
       <c r="CR6" s="104" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="CS6" s="104">
         <v>60.2</v>
@@ -11463,7 +11463,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -11472,83 +11472,83 @@
         <v>142</v>
       </c>
       <c r="G7" s="107" t="s">
-        <v>1051</v>
+        <v>1041</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="97" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="K7" s="97" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="L7" s="79" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="M7" s="106" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="N7" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="O7" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="P7" s="107" t="s">
-        <v>1054</v>
+        <v>1044</v>
       </c>
       <c r="Q7" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="R7" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="S7" s="115" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="T7" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="U7" s="107"/>
       <c r="V7" s="117" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
       <c r="W7" s="117" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="X7" s="97"/>
       <c r="Y7" s="106" t="s">
-        <v>977</v>
+        <v>967</v>
       </c>
       <c r="Z7" s="97" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="AA7" s="107"/>
       <c r="AB7" s="107" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AC7" s="107" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="AD7" s="97" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="AE7" s="107"/>
       <c r="AF7" s="107" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AG7" s="106" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AH7" s="107" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="AI7" s="107"/>
       <c r="AJ7" s="97"/>
       <c r="AM7" s="107"/>
       <c r="AN7" s="107"/>
       <c r="AO7" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="AP7" s="50"/>
       <c r="AQ7" s="50"/>
@@ -11557,16 +11557,16 @@
         <v>1</v>
       </c>
       <c r="AT7" s="80" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="AU7" s="107">
         <v>3</v>
       </c>
       <c r="AV7" s="107" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AW7" s="107" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="AX7" s="107" t="s">
         <v>143</v>
@@ -11575,58 +11575,58 @@
         <v>140</v>
       </c>
       <c r="AZ7" s="107" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="BA7" s="107">
         <v>2</v>
       </c>
       <c r="BB7" s="107" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="BC7" s="107">
         <v>3</v>
       </c>
       <c r="BD7" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="BE7" s="107" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="BF7" s="107" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="BG7" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BH7" s="107" t="s">
-        <v>1067</v>
+        <v>1057</v>
       </c>
       <c r="BI7" s="106" t="s">
-        <v>1064</v>
+        <v>1054</v>
       </c>
       <c r="BJ7" s="107" t="s">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="BK7" s="74" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="BL7" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="BM7" s="107"/>
       <c r="BN7" s="107" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="BO7" s="117" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="BP7" s="97"/>
       <c r="BQ7" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BR7" s="107"/>
       <c r="BS7" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BT7" s="107"/>
       <c r="BU7" s="106">
@@ -11639,7 +11639,7 @@
         <v>2</v>
       </c>
       <c r="BX7" s="37" t="s">
-        <v>993</v>
+        <v>983</v>
       </c>
       <c r="BY7" s="4"/>
       <c r="BZ7" s="5"/>
@@ -11650,10 +11650,10 @@
       <c r="CE7" s="5"/>
       <c r="CF7" s="5"/>
       <c r="CG7" s="42" t="s">
-        <v>994</v>
+        <v>984</v>
       </c>
       <c r="CH7" s="43" t="s">
-        <v>995</v>
+        <v>985</v>
       </c>
       <c r="CI7" s="43"/>
       <c r="CJ7" s="43">
@@ -11664,20 +11664,20 @@
       </c>
       <c r="CL7" s="43"/>
       <c r="CM7" s="4" t="s">
-        <v>1001</v>
+        <v>991</v>
       </c>
       <c r="CN7" s="61">
         <v>1.0900000000000001</v>
       </c>
       <c r="CO7" s="67" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="CP7" s="5"/>
       <c r="CQ7" s="4">
         <v>3</v>
       </c>
       <c r="CR7" s="5" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="CS7" s="5">
         <v>50.2</v>
@@ -11755,7 +11755,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="E8" s="106">
         <v>2</v>
@@ -11764,76 +11764,76 @@
         <v>142</v>
       </c>
       <c r="G8" s="107" t="s">
-        <v>1051</v>
+        <v>1041</v>
       </c>
       <c r="H8" s="107"/>
       <c r="I8" s="107"/>
       <c r="J8" s="97" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="K8" s="97" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="M8" s="106" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="N8" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="O8" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="P8" s="107" t="s">
-        <v>1054</v>
+        <v>1044</v>
       </c>
       <c r="Q8" s="107" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="R8" s="107" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="S8" s="115" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="T8" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="U8" s="107"/>
       <c r="V8" s="117" t="s">
-        <v>1055</v>
+        <v>1045</v>
       </c>
       <c r="W8" s="117" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="X8" s="97"/>
       <c r="Y8" s="106" t="s">
-        <v>977</v>
+        <v>967</v>
       </c>
       <c r="Z8" s="97" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="AA8" s="107"/>
       <c r="AB8" s="107" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AC8" s="107" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="AD8" s="97" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="AE8" s="107"/>
       <c r="AF8" s="107" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="AG8" s="106" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AH8" s="107" t="s">
-        <v>1044</v>
+        <v>1034</v>
       </c>
       <c r="AI8" s="107"/>
       <c r="AJ8" s="97"/>
@@ -11842,7 +11842,7 @@
       <c r="AM8" s="107"/>
       <c r="AN8" s="107"/>
       <c r="AO8" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="AP8" s="50"/>
       <c r="AQ8" s="50"/>
@@ -11851,16 +11851,16 @@
         <v>1</v>
       </c>
       <c r="AT8" s="80" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="AU8" s="107">
         <v>3</v>
       </c>
       <c r="AV8" s="107" t="s">
-        <v>1043</v>
+        <v>1033</v>
       </c>
       <c r="AW8" s="107" t="s">
-        <v>1045</v>
+        <v>1035</v>
       </c>
       <c r="AX8" s="107" t="s">
         <v>143</v>
@@ -11869,58 +11869,58 @@
         <v>140</v>
       </c>
       <c r="AZ8" s="107" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="BA8" s="107">
         <v>2</v>
       </c>
       <c r="BB8" s="107" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="BC8" s="107">
         <v>3</v>
       </c>
       <c r="BD8" s="107" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="BE8" s="107" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="BF8" s="107" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="BG8" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BH8" s="107" t="s">
-        <v>1067</v>
+        <v>1057</v>
       </c>
       <c r="BI8" s="106" t="s">
-        <v>1064</v>
+        <v>1054</v>
       </c>
       <c r="BJ8" s="107" t="s">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="BK8" s="74" t="s">
-        <v>1047</v>
+        <v>1037</v>
       </c>
       <c r="BL8" s="116" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="BM8" s="107"/>
       <c r="BN8" s="107" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="BO8" s="117" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="BP8" s="97"/>
       <c r="BQ8" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BR8" s="107"/>
       <c r="BS8" s="107" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="BT8" s="107"/>
       <c r="BU8" s="106">
@@ -11933,7 +11933,7 @@
         <v>2</v>
       </c>
       <c r="BX8" s="37" t="s">
-        <v>993</v>
+        <v>983</v>
       </c>
       <c r="BY8" s="106"/>
       <c r="BZ8" s="107"/>
@@ -11944,10 +11944,10 @@
       <c r="CE8" s="107"/>
       <c r="CF8" s="107"/>
       <c r="CG8" s="42" t="s">
-        <v>994</v>
+        <v>984</v>
       </c>
       <c r="CH8" s="78" t="s">
-        <v>995</v>
+        <v>985</v>
       </c>
       <c r="CI8" s="78"/>
       <c r="CJ8" s="78">
@@ -11958,20 +11958,20 @@
       </c>
       <c r="CL8" s="78"/>
       <c r="CM8" s="106" t="s">
-        <v>1001</v>
+        <v>991</v>
       </c>
       <c r="CN8" s="61">
         <v>1.0900000000000001</v>
       </c>
       <c r="CO8" s="106" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="CP8" s="107"/>
       <c r="CQ8" s="106">
         <v>4</v>
       </c>
       <c r="CR8" s="107" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
       <c r="CS8" s="107">
         <v>58.7</v>
@@ -34909,7 +34909,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="20" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
@@ -34917,13 +34917,13 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -35005,7 +35005,7 @@
         <v>447</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>790</v>
+        <v>780</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>446</v>
@@ -35115,7 +35115,7 @@
         <v>10</v>
       </c>
       <c r="R5" s="108" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="S5" s="108">
         <v>100</v>
@@ -35183,7 +35183,7 @@
         <v>10</v>
       </c>
       <c r="R6" s="109" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="S6" s="109">
         <v>100</v>
@@ -35232,7 +35232,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>988</v>
+        <v>978</v>
       </c>
       <c r="B1" s="111"/>
     </row>
@@ -35241,7 +35241,7 @@
         <v>641</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>989</v>
+        <v>979</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -35252,10 +35252,10 @@
     </row>
     <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
-        <v>990</v>
+        <v>980</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>991</v>
+        <v>981</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -35263,7 +35263,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>992</v>
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -35283,7 +35283,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
@@ -35291,13 +35291,13 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -35913,7 +35913,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
@@ -35921,19 +35921,19 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>778</v>
+        <v>768</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -36181,10 +36181,10 @@
         <v>377</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1170</v>
+        <v>1159</v>
       </c>
       <c r="L1" t="s">
-        <v>1169</v>
+        <v>1158</v>
       </c>
       <c r="N1" t="s">
         <v>383</v>
@@ -36193,14 +36193,14 @@
         <v>527</v>
       </c>
       <c r="S1" s="111" t="s">
-        <v>1155</v>
+        <v>1145</v>
       </c>
       <c r="T1" s="111"/>
       <c r="U1" s="111" t="s">
-        <v>1158</v>
+        <v>1148</v>
       </c>
       <c r="W1" s="111" t="s">
-        <v>1156</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -36229,14 +36229,14 @@
         <v>7</v>
       </c>
       <c r="S2" s="111" t="s">
-        <v>1157</v>
+        <v>1147</v>
       </c>
       <c r="T2" s="111"/>
       <c r="U2" s="111" t="s">
-        <v>1159</v>
+        <v>1149</v>
       </c>
       <c r="W2" s="131" t="s">
-        <v>1149</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -36265,14 +36265,14 @@
         <v>519</v>
       </c>
       <c r="S3" s="111" t="s">
-        <v>1147</v>
+        <v>1137</v>
       </c>
       <c r="T3" s="111"/>
       <c r="U3" s="111" t="s">
-        <v>1160</v>
+        <v>1150</v>
       </c>
       <c r="W3" s="131" t="s">
-        <v>1150</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -36298,11 +36298,11 @@
         <v>520</v>
       </c>
       <c r="S4" s="111" t="s">
-        <v>1148</v>
+        <v>1138</v>
       </c>
       <c r="T4" s="111"/>
       <c r="W4" s="131" t="s">
-        <v>1151</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -36429,7 +36429,7 @@
         <v>85</v>
       </c>
       <c r="K12" t="s">
-        <v>1165</v>
+        <v>1155</v>
       </c>
       <c r="L12" t="s">
         <v>56</v>
@@ -36536,7 +36536,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="20" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -36544,7 +36544,7 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>637</v>
@@ -36640,10 +36640,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
     </row>
   </sheetData>
@@ -36656,7 +36656,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36680,7 +36680,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="20" customFormat="1" ht="299.25" x14ac:dyDescent="0.25">
@@ -36700,13 +36700,13 @@
         <v>655</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>656</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>1167</v>
+        <v>1156</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>657</v>
@@ -36721,10 +36721,10 @@
         <v>660</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -36794,7 +36794,7 @@
         <v>336</v>
       </c>
       <c r="H4" s="70" t="s">
-        <v>1168</v>
+        <v>1157</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>337</v>
@@ -36827,26 +36827,26 @@
         <v>1</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="E5" s="65">
         <v>1</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>1032</v>
+        <v>1022</v>
       </c>
       <c r="H5" s="66"/>
       <c r="I5" s="65" t="s">
         <v>95</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>1038</v>
+        <v>1028</v>
       </c>
       <c r="K5" s="111" t="s">
-        <v>1038</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -36860,26 +36860,26 @@
         <v>1</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="E6" s="65">
         <v>1</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="G6" s="66" t="s">
-        <v>1033</v>
+        <v>1023</v>
       </c>
       <c r="H6" s="66"/>
       <c r="I6" s="111" t="s">
         <v>95</v>
       </c>
       <c r="J6" s="111" t="s">
-        <v>1048</v>
+        <v>1038</v>
       </c>
       <c r="K6" s="111" t="s">
-        <v>1048</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -37085,7 +37085,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="20" customFormat="1" ht="174" thickBot="1" x14ac:dyDescent="0.3">
@@ -37096,40 +37096,40 @@
         <v>642</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>913</v>
+        <v>903</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>914</v>
+        <v>904</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>643</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="O2" s="20" t="s">
         <v>644</v>
@@ -37138,7 +37138,7 @@
         <v>645</v>
       </c>
       <c r="Q2" s="75" t="s">
-        <v>939</v>
+        <v>929</v>
       </c>
       <c r="R2" s="20" t="s">
         <v>646</v>
@@ -37206,10 +37206,10 @@
         <v>340</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>341</v>
@@ -37245,7 +37245,7 @@
         <v>350</v>
       </c>
       <c r="Q4" s="70" t="s">
-        <v>940</v>
+        <v>930</v>
       </c>
       <c r="R4" s="7" t="s">
         <v>351</v>
@@ -37265,7 +37265,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="H5" s="65" t="s">
         <v>85</v>
@@ -37274,23 +37274,23 @@
         <v>1</v>
       </c>
       <c r="L5" s="65" t="s">
-        <v>922</v>
+        <v>912</v>
       </c>
       <c r="M5" s="65" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>923</v>
+        <v>913</v>
       </c>
       <c r="O5" s="65" t="s">
-        <v>924</v>
+        <v>914</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>925</v>
+        <v>915</v>
       </c>
       <c r="Q5" s="82"/>
       <c r="R5" s="66" t="s">
-        <v>926</v>
+        <v>916</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -37307,7 +37307,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="65" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="H6" s="65" t="s">
         <v>85</v>
@@ -37316,23 +37316,23 @@
         <v>2</v>
       </c>
       <c r="L6" s="65" t="s">
-        <v>922</v>
+        <v>912</v>
       </c>
       <c r="M6" s="65" t="s">
         <v>25</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
       <c r="O6" s="65" t="s">
-        <v>924</v>
+        <v>914</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>928</v>
+        <v>918</v>
       </c>
       <c r="Q6" s="82"/>
       <c r="R6" s="66" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -37392,7 +37392,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="20" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
@@ -37403,7 +37403,7 @@
         <v>647</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>648</v>
@@ -37472,17 +37472,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="D5" s="65" t="s">
         <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="F5" s="65"/>
       <c r="G5" s="66" t="s">
-        <v>932</v>
+        <v>922</v>
       </c>
       <c r="H5" s="56"/>
     </row>
@@ -37494,17 +37494,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>933</v>
+        <v>923</v>
       </c>
       <c r="D6" s="65" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="F6" s="65"/>
       <c r="G6" s="66" t="s">
-        <v>934</v>
+        <v>924</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -37515,17 +37515,17 @@
         <v>1</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>935</v>
+        <v>925</v>
       </c>
       <c r="D7" s="65" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="F7" s="65"/>
       <c r="G7" s="66" t="s">
-        <v>936</v>
+        <v>926</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -37536,17 +37536,17 @@
         <v>2</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>937</v>
+        <v>927</v>
       </c>
       <c r="D8" s="65" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="F8" s="65"/>
       <c r="G8" s="66" t="s">
-        <v>938</v>
+        <v>928</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -38118,7 +38118,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:XFD4"/>
+      <selection activeCell="F31" sqref="F31:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -38130,7 +38130,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="20" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -38168,7 +38168,7 @@
         <v>493</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>1078</v>
+        <v>1068</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>494</v>
@@ -38185,19 +38185,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>941</v>
+        <v>931</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>944</v>
+        <v>934</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>945</v>
+        <v>935</v>
       </c>
       <c r="G5" s="65">
         <v>1.1000000000000001</v>
@@ -38208,13 +38208,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>947</v>
+        <v>937</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>948</v>
+        <v>938</v>
       </c>
       <c r="E6" s="65"/>
       <c r="F6" s="65" t="s">
@@ -38352,28 +38352,28 @@
         <v>641</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>663</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>664</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>666</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>667</v>
@@ -38391,10 +38391,10 @@
         <v>671</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="Q2" s="20" t="s">
         <v>672</v>
@@ -38406,7 +38406,7 @@
         <v>674</v>
       </c>
       <c r="T2" s="75" t="s">
-        <v>1002</v>
+        <v>992</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -38468,7 +38468,7 @@
         <v>107</v>
       </c>
       <c r="T3" s="87" t="s">
-        <v>1003</v>
+        <v>993</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -38538,7 +38538,7 @@
         <v>381</v>
       </c>
       <c r="T4" s="70" t="s">
-        <v>1004</v>
+        <v>994</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
@@ -38546,13 +38546,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>949</v>
+        <v>939</v>
       </c>
       <c r="E5" s="65">
         <v>1</v>
@@ -38564,32 +38564,32 @@
         <v>1</v>
       </c>
       <c r="H5" s="65" t="s">
-        <v>1034</v>
+        <v>1024</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>1035</v>
+        <v>1025</v>
       </c>
       <c r="J5" s="65">
         <v>1</v>
       </c>
       <c r="K5" s="65" t="s">
-        <v>950</v>
+        <v>940</v>
       </c>
       <c r="L5" s="65" t="s">
-        <v>951</v>
+        <v>941</v>
       </c>
       <c r="M5" s="65" t="s">
-        <v>952</v>
+        <v>942</v>
       </c>
       <c r="N5" s="65"/>
       <c r="O5" s="65" t="s">
-        <v>1036</v>
+        <v>1026</v>
       </c>
       <c r="P5" s="65" t="s">
-        <v>953</v>
+        <v>943</v>
       </c>
       <c r="Q5" s="65" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="R5" s="65">
         <v>0</v>
@@ -38603,13 +38603,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="C6" s="65">
         <v>2</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>949</v>
+        <v>939</v>
       </c>
       <c r="E6" s="65">
         <v>1</v>
@@ -38621,32 +38621,32 @@
         <v>1</v>
       </c>
       <c r="H6" s="111" t="s">
-        <v>1034</v>
+        <v>1024</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1035</v>
+        <v>1025</v>
       </c>
       <c r="J6" s="65">
         <v>1</v>
       </c>
       <c r="K6" s="65" t="s">
-        <v>950</v>
+        <v>940</v>
       </c>
       <c r="L6" s="65" t="s">
-        <v>951</v>
+        <v>941</v>
       </c>
       <c r="M6" s="65" t="s">
-        <v>952</v>
+        <v>942</v>
       </c>
       <c r="N6" s="65"/>
       <c r="O6" s="65" t="s">
-        <v>1037</v>
+        <v>1027</v>
       </c>
       <c r="P6" s="65" t="s">
-        <v>953</v>
+        <v>943</v>
       </c>
       <c r="Q6" s="65" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="R6" s="65">
         <v>0</v>
@@ -38778,31 +38778,31 @@
         <v>662</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>741</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>743</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>745</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>747</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>748</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>749</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>750</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>751</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>753</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>754</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>755</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>756</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="78.75" hidden="1" x14ac:dyDescent="0.25">
@@ -38889,7 +38889,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -38898,7 +38898,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -38921,7 +38921,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -38930,7 +38930,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="G6">
         <v>1</v>

</xml_diff>

<commit_message>
Unify naming of tabs in spreadsheet
Unify naming of tabs in spreadsheet w.r.t. underscores vs. tabs. Old names vs. new names: "Multi-state modeling" => "Multi_state_modeling"; "Multi-state scheme" => "Multi_state_scheme"; "Collection of models" => "Collection_of_models"
</commit_message>
<xml_diff>
--- a/example/xls_example.xlsx
+++ b/example/xls_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\flr2mmcif_development\20240619_update_excel_sheet\flr2mmcif\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\flr2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEA03A9-E4BA-43DD-AABE-1A9E3F4971D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C6FBB7-B81B-4349-927D-25AC52FF242D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
     <sheet name="Starting_comparative_model" sheetId="16" r:id="rId9"/>
     <sheet name="Modeling_protocol" sheetId="6" r:id="rId10"/>
     <sheet name="Modeling_post_process" sheetId="15" r:id="rId11"/>
-    <sheet name="Multi-state modeling" sheetId="7" r:id="rId12"/>
-    <sheet name="Multi-state scheme" sheetId="22" r:id="rId13"/>
+    <sheet name="Multi_state_modeling" sheetId="7" r:id="rId12"/>
+    <sheet name="Multi_state_scheme" sheetId="22" r:id="rId13"/>
     <sheet name="Models" sheetId="2" r:id="rId14"/>
-    <sheet name="Collection of models" sheetId="17" r:id="rId15"/>
+    <sheet name="Collection_of_models" sheetId="17" r:id="rId15"/>
     <sheet name="Reference_measurements" sheetId="20" r:id="rId16"/>
     <sheet name="FLR" sheetId="8" r:id="rId17"/>
     <sheet name="FLR_FPS_MPP_group" sheetId="18" r:id="rId18"/>
@@ -71,8 +71,8 @@
     <definedName name="Software_id">Software!$A$5:$A$1048576</definedName>
     <definedName name="solvent_phase_enumeration">for_internal_use_only!$E$2:$E$4</definedName>
     <definedName name="starting_model_id">Instance!$O$5:$O$1048576</definedName>
-    <definedName name="State_id">'Multi-state modeling'!$B$5:$B$1048576</definedName>
-    <definedName name="State_name">'Multi-state modeling'!$G$5:$G$1048576</definedName>
+    <definedName name="State_id">Multi_state_modeling!$B$5:$B$1048576</definedName>
+    <definedName name="State_name">Multi_state_modeling!$G$5:$G$1048576</definedName>
     <definedName name="structure_assembly_id">Instance!$G$5:$G$1048576</definedName>
     <definedName name="Yes_no_selection">for_internal_use_only!$A$2:$A$3</definedName>
   </definedNames>
@@ -4576,7 +4576,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>